<commit_message>
fixed 3rd future inclusion
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YCSTDBootstrapping.xlsx
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="147">
   <si>
     <t>60Y</t>
   </si>
@@ -515,156 +515,6 @@
     <t>General Settings</t>
   </si>
   <si>
-    <t>EUR_YCSTDRH_OND</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_TND</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_SND</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_SWD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_2WD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_3WD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_1MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_2MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_3MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_4MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_5MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_6MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_7MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_8MD</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_FUT3MH5</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_FUT3MM5</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_FUT3MU5</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_FUT3MZ5</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E3Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E4Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E5Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E6Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E7Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E8Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E9Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E10Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E11Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E12Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E13Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E14Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E15Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E16Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E17Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E18Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E19Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E20Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E21Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E22Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E23Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E24Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E25Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E26Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E27Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E28Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E29Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E30Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E35Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E40Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E50Y</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_AB6E60Y</t>
-  </si>
-  <si>
     <t>9M</t>
   </si>
   <si>
@@ -804,12 +654,6 @@
   </si>
   <si>
     <t>EUR_YCRH_Swaps</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_FUT3MU4</t>
-  </si>
-  <si>
-    <t>EUR_YCSTDRH_FUT3MZ4</t>
   </si>
   <si>
     <t>EURSTD</t>
@@ -2315,7 +2159,7 @@
       <c r="E2" s="216"/>
       <c r="F2" s="217"/>
       <c r="H2" s="215" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="I2" s="216"/>
       <c r="J2" s="216"/>
@@ -2344,7 +2188,7 @@
       <c r="F4" s="60"/>
       <c r="H4" s="133"/>
       <c r="I4" s="132" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="J4" s="126" t="b">
         <v>1</v>
@@ -2363,7 +2207,7 @@
       <c r="F5" s="60"/>
       <c r="H5" s="133"/>
       <c r="I5" s="132" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="J5" s="134" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
@@ -2384,7 +2228,7 @@
       <c r="F6" s="60"/>
       <c r="H6" s="133"/>
       <c r="I6" s="132" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="J6" s="123" t="b">
         <v>1</v>
@@ -2433,7 +2277,7 @@
       <c r="E9" s="61"/>
       <c r="F9" s="60"/>
       <c r="H9" s="215" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="I9" s="216"/>
       <c r="J9" s="216"/>
@@ -2464,10 +2308,10 @@
       <c r="F11" s="60"/>
       <c r="H11" s="125"/>
       <c r="I11" s="124" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="J11" s="126" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="K11" s="122"/>
     </row>
@@ -2483,10 +2327,10 @@
       <c r="F12" s="60"/>
       <c r="H12" s="125"/>
       <c r="I12" s="124" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="J12" s="123" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="K12" s="122"/>
     </row>
@@ -2498,7 +2342,7 @@
       <c r="F13" s="60"/>
       <c r="H13" s="125"/>
       <c r="I13" s="124" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="J13" s="126" t="str">
         <f>PROPER(Currency)&amp;"YC"</f>
@@ -2513,13 +2357,13 @@
       </c>
       <c r="D14" s="81" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYCSTD#0002</v>
+        <v>_EURYCSTD#0006</v>
       </c>
       <c r="E14" s="61"/>
       <c r="F14" s="60"/>
       <c r="H14" s="125"/>
       <c r="I14" s="124" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="J14" s="126" t="str">
         <f>PROPER(Currency)&amp;"YCSTD"</f>
@@ -2540,10 +2384,10 @@
       <c r="F15" s="60"/>
       <c r="H15" s="207"/>
       <c r="I15" s="208" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="J15" s="209" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="K15" s="210"/>
     </row>
@@ -2562,10 +2406,10 @@
       <c r="F16" s="60"/>
       <c r="H16" s="207"/>
       <c r="I16" s="208" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="J16" s="209" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="K16" s="210"/>
     </row>
@@ -2641,7 +2485,7 @@
       </c>
       <c r="D23" s="67">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>2.5733868722344396E-2</v>
+        <v>2.5793399729359772E-2</v>
       </c>
       <c r="E23" s="61"/>
       <c r="F23" s="60"/>
@@ -2654,7 +2498,7 @@
       </c>
       <c r="D24" s="65">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>1.520830164926483E-3</v>
+        <v>1.3180531757461815E-3</v>
       </c>
       <c r="E24" s="61"/>
       <c r="F24" s="60"/>
@@ -2674,7 +2518,7 @@
     <row r="26" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="59"/>
       <c r="C26" s="58" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="D26" s="58" t="b">
         <f>_xll.qlRelinkableHandleLinkTo(C26,YieldCurve)</f>
@@ -2725,7 +2569,7 @@
   <dimension ref="A1:R166"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2791,7 +2635,7 @@
       </c>
       <c r="F2" s="13">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="12" t="b">
@@ -2861,7 +2705,7 @@
       </c>
       <c r="F4" s="13">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>1.8E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="12" t="b">
@@ -3130,11 +2974,11 @@
       </c>
       <c r="O11" s="29">
         <f>_xll.qlYieldTSForwardRate(YieldCurve,K2,L124,"act/365","simple","annual")</f>
-        <v>3.7630918750955818E-2</v>
+        <v>3.7670999009817858E-2</v>
       </c>
       <c r="Q11" s="31">
         <f>_xll.qlYieldTSDiscount(YieldCurve,L124)</f>
-        <v>0.47812509770083361</v>
+        <v>0.47785948287253094</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
@@ -3210,7 +3054,7 @@
       </c>
       <c r="Q13" s="31">
         <f>1/Q11</f>
-        <v>2.0915028405927925</v>
+        <v>2.0926653877176484</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
@@ -3298,11 +3142,11 @@
       </c>
       <c r="Q15" s="29">
         <f>(Q13^(1/Q14))-1</f>
-        <v>2.5748531871447433E-2</v>
+        <v>2.5768170420287451E-2</v>
       </c>
       <c r="R15" s="29">
         <f>(Q13-1)/Q14</f>
-        <v>3.7606054069885715E-2</v>
+        <v>3.7646107845661851E-2</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
@@ -4012,7 +3856,7 @@
       </c>
       <c r="F34" s="28">
         <f>_xll.qlRateHelperQuoteValue($E34,Trigger)</f>
-        <v>99.747500000000002</v>
+        <v>99.75</v>
       </c>
       <c r="G34" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E34,Trigger)</f>
@@ -4054,7 +3898,7 @@
       </c>
       <c r="F35" s="28">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
-        <v>99.757499999999993</v>
+        <v>99.754999999999995</v>
       </c>
       <c r="G35" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E35,Trigger)</f>
@@ -4096,7 +3940,7 @@
       </c>
       <c r="F36" s="28">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
-        <v>99.752499999999998</v>
+        <v>99.757499999999993</v>
       </c>
       <c r="G36" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E36,Trigger)</f>
@@ -4222,14 +4066,14 @@
       </c>
       <c r="F39" s="28">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
-        <v>99.747500000000002</v>
+        <v>99.752499999999998</v>
       </c>
       <c r="G39" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E39,Trigger)</f>
         <v>0</v>
       </c>
       <c r="H39" s="212" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="12">
         <v>60</v>
@@ -4313,7 +4157,7 @@
         <v>#NUM!</v>
       </c>
       <c r="H41" s="212" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="12">
         <v>60</v>
@@ -4348,14 +4192,14 @@
       </c>
       <c r="F42" s="28">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
-        <v>99.727499999999992</v>
+        <v>99.732500000000002</v>
       </c>
       <c r="G42" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E42,Trigger)</f>
         <v>0</v>
       </c>
       <c r="H42" s="212" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="12">
         <v>60</v>
@@ -4439,7 +4283,7 @@
         <v>#NUM!</v>
       </c>
       <c r="H44" s="212" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="12">
         <v>60</v>
@@ -4474,7 +4318,7 @@
       </c>
       <c r="F45" s="28">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
-        <v>99.697499999999991</v>
+        <v>99.702500000000001</v>
       </c>
       <c r="G45" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E45,Trigger)</f>
@@ -4516,13 +4360,13 @@
       </c>
       <c r="F46" s="28">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
-        <v>99.657499999999999</v>
+        <v>99.662499999999994</v>
       </c>
       <c r="G46" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E46,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="12" t="b">
+      <c r="H46" s="212" t="b">
         <v>1</v>
       </c>
       <c r="I46" s="12">
@@ -4558,13 +4402,13 @@
       </c>
       <c r="F47" s="28">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
-        <v>99.602499999999992</v>
+        <v>99.607500000000002</v>
       </c>
       <c r="G47" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E47,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="12" t="b">
+      <c r="H47" s="212" t="b">
         <v>1</v>
       </c>
       <c r="I47" s="12">
@@ -4600,13 +4444,13 @@
       </c>
       <c r="F48" s="28">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
-        <v>99.527500000000003</v>
+        <v>99.537499999999994</v>
       </c>
       <c r="G48" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E48,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="H48" s="12" t="b">
+      <c r="H48" s="212" t="b">
         <v>1</v>
       </c>
       <c r="I48" s="12">
@@ -4642,13 +4486,13 @@
       </c>
       <c r="F49" s="28">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
-        <v>99.4375</v>
+        <v>99.442499999999995</v>
       </c>
       <c r="G49" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E49,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="H49" s="12" t="b">
+      <c r="H49" s="212" t="b">
         <v>1</v>
       </c>
       <c r="I49" s="12">
@@ -4684,13 +4528,13 @@
       </c>
       <c r="F50" s="28">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
-        <v>99.327500000000001</v>
+        <v>99.337500000000006</v>
       </c>
       <c r="G50" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E50,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="H50" s="12" t="b">
+      <c r="H50" s="212" t="b">
         <v>1</v>
       </c>
       <c r="I50" s="12">
@@ -4726,13 +4570,13 @@
       </c>
       <c r="F51" s="28">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
-        <v>99.197499999999991</v>
+        <v>99.207499999999996</v>
       </c>
       <c r="G51" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E51,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="H51" s="12" t="b">
+      <c r="H51" s="212" t="b">
         <v>1</v>
       </c>
       <c r="I51" s="12">
@@ -4768,7 +4612,7 @@
       </c>
       <c r="F52" s="28">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
-        <v>99.064999999999998</v>
+        <v>99.072499999999991</v>
       </c>
       <c r="G52" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E52,Trigger)</f>
@@ -4810,7 +4654,7 @@
       </c>
       <c r="F53" s="28">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
-        <v>98.9375</v>
+        <v>98.947499999999991</v>
       </c>
       <c r="G53" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E53,Trigger)</f>
@@ -4852,7 +4696,7 @@
       </c>
       <c r="F54" s="28">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
-        <v>98.802500000000009</v>
+        <v>98.814999999999998</v>
       </c>
       <c r="G54" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E54,Trigger)</f>
@@ -4894,7 +4738,7 @@
       </c>
       <c r="F55" s="28">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
-        <v>98.677500000000009</v>
+        <v>98.69</v>
       </c>
       <c r="G55" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E55,Trigger)</f>
@@ -4936,7 +4780,7 @@
       </c>
       <c r="F56" s="28">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
-        <v>98.552500000000009</v>
+        <v>98.567499999999995</v>
       </c>
       <c r="G56" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E56,Trigger)</f>
@@ -4978,7 +4822,7 @@
       </c>
       <c r="F57" s="28">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
-        <v>98.444999999999993</v>
+        <v>98.460000000000008</v>
       </c>
       <c r="G57" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E57,Trigger)</f>
@@ -5020,7 +4864,7 @@
       </c>
       <c r="F58" s="28">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
-        <v>98.337500000000006</v>
+        <v>98.35</v>
       </c>
       <c r="G58" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E58,Trigger)</f>
@@ -5062,7 +4906,7 @@
       </c>
       <c r="F59" s="28">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
-        <v>98.234999999999999</v>
+        <v>98.247500000000002</v>
       </c>
       <c r="G59" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E59,Trigger)</f>
@@ -5104,7 +4948,7 @@
       </c>
       <c r="F60" s="28">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
-        <v>98.12</v>
+        <v>98.127499999999998</v>
       </c>
       <c r="G60" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E60,Trigger)</f>
@@ -5146,7 +4990,7 @@
       </c>
       <c r="F61" s="28">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
-        <v>98.012500000000003</v>
+        <v>98.022500000000008</v>
       </c>
       <c r="G61" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E61,Trigger)</f>
@@ -5188,7 +5032,7 @@
       </c>
       <c r="F62" s="28">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
-        <v>97.914999999999992</v>
+        <v>97.92</v>
       </c>
       <c r="G62" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E62,Trigger)</f>
@@ -5230,7 +5074,7 @@
       </c>
       <c r="F63" s="28">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>97.814999999999998</v>
+        <v>97.82</v>
       </c>
       <c r="G63" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E63,Trigger)</f>
@@ -5272,7 +5116,7 @@
       </c>
       <c r="F64" s="28">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
-        <v>97.715000000000003</v>
+        <v>97.72</v>
       </c>
       <c r="G64" s="13">
         <f>_xll.qlFuturesRateHelperConvexityAdjustment($E64,Trigger)</f>
@@ -6421,7 +6265,7 @@
       </c>
       <c r="F93" s="13">
         <f>_xll.qlRateHelperQuoteValue($E93,Trigger)</f>
-        <v>3.8500000000000001E-3</v>
+        <v>3.81E-3</v>
       </c>
       <c r="G93" s="13">
         <f>_xll.qlSwapRateHelperSpread($E93,Trigger)</f>
@@ -6467,7 +6311,7 @@
       </c>
       <c r="F94" s="13">
         <f>_xll.qlRateHelperQuoteValue($E94,Trigger)</f>
-        <v>3.7000000000000002E-3</v>
+        <v>3.64E-3</v>
       </c>
       <c r="G94" s="13">
         <f>_xll.qlSwapRateHelperSpread($E94,Trigger)</f>
@@ -6513,7 +6357,7 @@
       </c>
       <c r="F95" s="13">
         <f>_xll.qlRateHelperQuoteValue($E95,Trigger)</f>
-        <v>4.1200000000000004E-3</v>
+        <v>4.0600000000000002E-3</v>
       </c>
       <c r="G95" s="13">
         <f>_xll.qlSwapRateHelperSpread($E95,Trigger)</f>
@@ -6559,7 +6403,7 @@
       </c>
       <c r="F96" s="13">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
-        <v>4.1099999999999999E-3</v>
+        <v>4.0400000000000002E-3</v>
       </c>
       <c r="G96" s="13">
         <f>_xll.qlSwapRateHelperSpread($E96,Trigger)</f>
@@ -6605,7 +6449,7 @@
       </c>
       <c r="F97" s="13">
         <f>_xll.qlRateHelperQuoteValue($E97,Trigger)</f>
-        <v>4.5199999999999997E-3</v>
+        <v>4.4600000000000004E-3</v>
       </c>
       <c r="G97" s="13">
         <f>_xll.qlSwapRateHelperSpread($E97,Trigger)</f>
@@ -6651,7 +6495,7 @@
       </c>
       <c r="F98" s="13">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
-        <v>5.9699999999999996E-3</v>
+        <v>5.8899999999999994E-3</v>
       </c>
       <c r="G98" s="13">
         <f>_xll.qlSwapRateHelperSpread($E98,Trigger)</f>
@@ -6697,7 +6541,7 @@
       </c>
       <c r="F99" s="13">
         <f>_xll.qlRateHelperQuoteValue($E99,Trigger)</f>
-        <v>7.9000000000000008E-3</v>
+        <v>7.8100000000000001E-3</v>
       </c>
       <c r="G99" s="13">
         <f>_xll.qlSwapRateHelperSpread($E99,Trigger)</f>
@@ -6743,7 +6587,7 @@
       </c>
       <c r="F100" s="13">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
-        <v>9.9299999999999996E-3</v>
+        <v>9.8399999999999998E-3</v>
       </c>
       <c r="G100" s="13">
         <f>_xll.qlSwapRateHelperSpread($E100,Trigger)</f>
@@ -6789,7 +6633,7 @@
       </c>
       <c r="F101" s="13">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
-        <v>1.191E-2</v>
+        <v>1.183E-2</v>
       </c>
       <c r="G101" s="13">
         <f>_xll.qlSwapRateHelperSpread($E101,Trigger)</f>
@@ -6835,7 +6679,7 @@
       </c>
       <c r="F102" s="13">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
-        <v>1.376E-2</v>
+        <v>1.37E-2</v>
       </c>
       <c r="G102" s="13">
         <f>_xll.qlSwapRateHelperSpread($E102,Trigger)</f>
@@ -6881,7 +6725,7 @@
       </c>
       <c r="F103" s="13">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
-        <v>1.5449999999999998E-2</v>
+        <v>1.541E-2</v>
       </c>
       <c r="G103" s="13">
         <f>_xll.qlSwapRateHelperSpread($E103,Trigger)</f>
@@ -6927,7 +6771,7 @@
       </c>
       <c r="F104" s="13">
         <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
-        <v>1.6969999999999999E-2</v>
+        <v>1.695E-2</v>
       </c>
       <c r="G104" s="13">
         <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
@@ -6973,7 +6817,7 @@
       </c>
       <c r="F105" s="13">
         <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>1.8340000000000002E-2</v>
+        <v>1.8319999999999999E-2</v>
       </c>
       <c r="G105" s="13">
         <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
@@ -7019,7 +6863,7 @@
       </c>
       <c r="F106" s="13">
         <f>_xll.qlRateHelperQuoteValue($E106,Trigger)</f>
-        <v>1.9530000000000002E-2</v>
+        <v>1.951E-2</v>
       </c>
       <c r="G106" s="13">
         <f>_xll.qlSwapRateHelperSpread($E106,Trigger)</f>
@@ -7157,7 +7001,7 @@
       </c>
       <c r="F109" s="13">
         <f>_xll.qlRateHelperQuoteValue($E109,Trigger)</f>
-        <v>2.2160000000000003E-2</v>
+        <v>2.2170000000000002E-2</v>
       </c>
       <c r="G109" s="13">
         <f>_xll.qlSwapRateHelperSpread($E109,Trigger)</f>
@@ -7203,7 +7047,7 @@
       </c>
       <c r="F110" s="13">
         <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>2.2759999999999999E-2</v>
+        <v>2.2770000000000002E-2</v>
       </c>
       <c r="G110" s="13">
         <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
@@ -7249,7 +7093,7 @@
       </c>
       <c r="F111" s="13">
         <f>_xll.qlRateHelperQuoteValue($E111,Trigger)</f>
-        <v>2.3239999999999997E-2</v>
+        <v>2.3250000000000003E-2</v>
       </c>
       <c r="G111" s="13">
         <f>_xll.qlSwapRateHelperSpread($E111,Trigger)</f>
@@ -7295,7 +7139,7 @@
       </c>
       <c r="F112" s="13">
         <f>_xll.qlRateHelperQuoteValue($E112,Trigger)</f>
-        <v>2.3620000000000002E-2</v>
+        <v>2.3629999999999998E-2</v>
       </c>
       <c r="G112" s="13">
         <f>_xll.qlSwapRateHelperSpread($E112,Trigger)</f>
@@ -7341,7 +7185,7 @@
       </c>
       <c r="F113" s="13">
         <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>2.392E-2</v>
+        <v>2.3929999999999996E-2</v>
       </c>
       <c r="G113" s="13">
         <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
@@ -7387,7 +7231,7 @@
       </c>
       <c r="F114" s="13">
         <f>_xll.qlRateHelperQuoteValue($E114,Trigger)</f>
-        <v>2.4140000000000002E-2</v>
+        <v>2.4150000000000001E-2</v>
       </c>
       <c r="G114" s="13">
         <f>_xll.qlSwapRateHelperSpread($E114,Trigger)</f>
@@ -7433,7 +7277,7 @@
       </c>
       <c r="F115" s="13">
         <f>_xll.qlRateHelperQuoteValue($E115,Trigger)</f>
-        <v>2.4310000000000002E-2</v>
+        <v>2.4319999999999998E-2</v>
       </c>
       <c r="G115" s="13">
         <f>_xll.qlSwapRateHelperSpread($E115,Trigger)</f>
@@ -7479,7 +7323,7 @@
       </c>
       <c r="F116" s="13">
         <f>_xll.qlRateHelperQuoteValue($E116,Trigger)</f>
-        <v>2.445E-2</v>
+        <v>2.4460000000000003E-2</v>
       </c>
       <c r="G116" s="13">
         <f>_xll.qlSwapRateHelperSpread($E116,Trigger)</f>
@@ -7525,7 +7369,7 @@
       </c>
       <c r="F117" s="13">
         <f>_xll.qlRateHelperQuoteValue($E117,Trigger)</f>
-        <v>2.4569999999999998E-2</v>
+        <v>2.4580000000000001E-2</v>
       </c>
       <c r="G117" s="13">
         <f>_xll.qlSwapRateHelperSpread($E117,Trigger)</f>
@@ -7571,7 +7415,7 @@
       </c>
       <c r="F118" s="13">
         <f>_xll.qlRateHelperQuoteValue($E118,Trigger)</f>
-        <v>2.4649999999999998E-2</v>
+        <v>2.4660000000000001E-2</v>
       </c>
       <c r="G118" s="13">
         <f>_xll.qlSwapRateHelperSpread($E118,Trigger)</f>
@@ -7617,7 +7461,7 @@
       </c>
       <c r="F119" s="13">
         <f>_xll.qlRateHelperQuoteValue($E119,Trigger)</f>
-        <v>2.4719999999999999E-2</v>
+        <v>2.4729999999999999E-2</v>
       </c>
       <c r="G119" s="13">
         <f>_xll.qlSwapRateHelperSpread($E119,Trigger)</f>
@@ -7663,7 +7507,7 @@
       </c>
       <c r="F120" s="13">
         <f>_xll.qlRateHelperQuoteValue($E120,Trigger)</f>
-        <v>2.4760000000000001E-2</v>
+        <v>2.477E-2</v>
       </c>
       <c r="G120" s="13">
         <f>_xll.qlSwapRateHelperSpread($E120,Trigger)</f>
@@ -7709,7 +7553,7 @@
       </c>
       <c r="F121" s="13">
         <f>_xll.qlRateHelperQuoteValue($E121,Trigger)</f>
-        <v>2.479E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="G121" s="13">
         <f>_xll.qlSwapRateHelperSpread($E121,Trigger)</f>
@@ -7755,7 +7599,7 @@
       </c>
       <c r="F122" s="13">
         <f>_xll.qlRateHelperQuoteValue($E122,Trigger)</f>
-        <v>2.4799999999999999E-2</v>
+        <v>2.4809999999999999E-2</v>
       </c>
       <c r="G122" s="13">
         <f>_xll.qlSwapRateHelperSpread($E122,Trigger)</f>
@@ -7847,7 +7691,7 @@
       </c>
       <c r="F124" s="13">
         <f>_xll.qlRateHelperQuoteValue($E124,Trigger)</f>
-        <v>2.4809999999999999E-2</v>
+        <v>2.4820000000000002E-2</v>
       </c>
       <c r="G124" s="13">
         <f>_xll.qlSwapRateHelperSpread($E124,Trigger)</f>
@@ -7893,7 +7737,7 @@
       </c>
       <c r="F125" s="13">
         <f>_xll.qlRateHelperQuoteValue($E125,Trigger)</f>
-        <v>2.4809999999999999E-2</v>
+        <v>2.4820000000000002E-2</v>
       </c>
       <c r="G125" s="13">
         <f>_xll.qlSwapRateHelperSpread($E125,Trigger)</f>
@@ -7939,7 +7783,7 @@
       </c>
       <c r="F126" s="13">
         <f>_xll.qlRateHelperQuoteValue($E126,Trigger)</f>
-        <v>2.4889999999999999E-2</v>
+        <v>2.4910000000000002E-2</v>
       </c>
       <c r="G126" s="13">
         <f>_xll.qlSwapRateHelperSpread($E126,Trigger)</f>
@@ -7985,7 +7829,7 @@
       </c>
       <c r="F127" s="13">
         <f>_xll.qlRateHelperQuoteValue($E127,Trigger)</f>
-        <v>2.5019999999999997E-2</v>
+        <v>2.5049999999999999E-2</v>
       </c>
       <c r="G127" s="13">
         <f>_xll.qlSwapRateHelperSpread($E127,Trigger)</f>
@@ -8031,7 +7875,7 @@
       </c>
       <c r="F128" s="13">
         <f>_xll.qlRateHelperQuoteValue($E128,Trigger)</f>
-        <v>2.5160000000000002E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="G128" s="13">
         <f>_xll.qlSwapRateHelperSpread($E128,Trigger)</f>
@@ -8077,7 +7921,7 @@
       </c>
       <c r="F129" s="6">
         <f>_xll.qlRateHelperQuoteValue($E129,Trigger)</f>
-        <v>2.529E-2</v>
+        <v>2.5329999999999998E-2</v>
       </c>
       <c r="G129" s="6">
         <f>_xll.qlSwapRateHelperSpread($E129,Trigger)</f>
@@ -9675,7 +9519,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -9690,7 +9534,7 @@
     <col min="7" max="8" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -9714,7 +9558,7 @@
       </c>
       <c r="I1" s="37">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>1.520830164926483E-3</v>
+        <v>1.3180531757461815E-3</v>
       </c>
       <c r="K1" s="211"/>
       <c r="L1" s="211"/>
@@ -9732,7 +9576,7 @@
       </c>
       <c r="E2" s="44">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F2" s="44" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -9747,14 +9591,13 @@
         <v>41703</v>
       </c>
       <c r="I2" s="37">
-        <v>1.520830164926483E-3</v>
-      </c>
-      <c r="K2" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" s="93">
-        <v>3.5000000000000001E-3</v>
-      </c>
+        <v>1.3180531757461815E-3</v>
+      </c>
+      <c r="K2" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D2,Trigger)</f>
+        <v>EUROND_Quote</v>
+      </c>
+      <c r="L2" s="93"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
@@ -9783,14 +9626,13 @@
         <v>41704</v>
       </c>
       <c r="I3" s="37">
-        <v>1.5715243911106976E-3</v>
-      </c>
-      <c r="K3" s="92" t="s">
-        <v>100</v>
-      </c>
-      <c r="L3" s="93">
-        <v>3.5000000000000001E-3</v>
-      </c>
+        <v>1.4701358965221966E-3</v>
+      </c>
+      <c r="K3" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D3,Trigger)</f>
+        <v>EURTND_Quote</v>
+      </c>
+      <c r="L3" s="93"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
@@ -9804,7 +9646,7 @@
       </c>
       <c r="E4" s="44">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>1.8E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="F4" s="44" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -9819,14 +9661,13 @@
         <v>41705</v>
       </c>
       <c r="I4" s="37">
-        <v>1.6560147399099533E-3</v>
-      </c>
-      <c r="K4" s="92" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" s="93">
-        <v>2.5000000000000001E-3</v>
-      </c>
+        <v>1.520830136596092E-3</v>
+      </c>
+      <c r="K4" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D4,Trigger)</f>
+        <v>EURSND_Quote</v>
+      </c>
+      <c r="L4" s="93"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
@@ -9855,14 +9696,13 @@
         <v>41711</v>
       </c>
       <c r="I5" s="37">
-        <v>1.7923038197417511E-3</v>
-      </c>
-      <c r="K5" s="92" t="s">
-        <v>102</v>
-      </c>
-      <c r="L5" s="93">
-        <v>1.949E-3</v>
-      </c>
+        <v>1.7697730431951958E-3</v>
+      </c>
+      <c r="K5" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D5,Trigger)</f>
+        <v>EuriborSWLastFixing_Quote</v>
+      </c>
+      <c r="L5" s="93"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="49" t="s">
@@ -9892,19 +9732,18 @@
         <v>41718</v>
       </c>
       <c r="I6" s="37">
-        <v>1.9174520182162202E-3</v>
-      </c>
-      <c r="K6" s="92" t="s">
-        <v>103</v>
-      </c>
-      <c r="L6" s="93">
-        <v>2.0590000000000001E-3</v>
-      </c>
+        <v>1.9047784563896743E-3</v>
+      </c>
+      <c r="K6" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D6,Trigger)</f>
+        <v>Euribor2WLastFixing_Quote</v>
+      </c>
+      <c r="L6" s="93"/>
     </row>
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_RateHelpersSelected#0002</v>
+        <v>EUR_YCSTDRH_RateHelpersSelected#0006</v>
       </c>
       <c r="B7" s="46" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -9930,14 +9769,13 @@
         <v>41736</v>
       </c>
       <c r="I7" s="37">
-        <v>2.1725025209642056E-3</v>
-      </c>
-      <c r="K7" s="92" t="s">
-        <v>104</v>
-      </c>
-      <c r="L7" s="93" t="e">
-        <v>#NUM!</v>
-      </c>
+        <v>2.166538491872436E-3</v>
+      </c>
+      <c r="K7" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D7,Trigger)</f>
+        <v>Euribor1MLastFixing_Quote</v>
+      </c>
+      <c r="L7" s="93"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D8" s="45" t="str">
@@ -9960,14 +9798,13 @@
         <v>41765</v>
       </c>
       <c r="I8" s="37">
-        <v>2.5036248352420885E-3</v>
-      </c>
-      <c r="K8" s="92" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="93">
-        <v>2.3800000000000002E-3</v>
-      </c>
+        <v>2.5004061528731991E-3</v>
+      </c>
+      <c r="K8" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D8,Trigger)</f>
+        <v>Euribor2MLastFixing_Quote</v>
+      </c>
+      <c r="L8" s="93"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="45" t="str">
@@ -9990,14 +9827,13 @@
         <v>41796</v>
       </c>
       <c r="I9" s="37">
-        <v>2.8803419658957434E-3</v>
-      </c>
-      <c r="K9" s="92" t="s">
-        <v>106</v>
-      </c>
-      <c r="L9" s="93">
-        <v>2.9949999999999998E-3</v>
-      </c>
+        <v>2.8781847638822957E-3</v>
+      </c>
+      <c r="K9" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D9,Trigger)</f>
+        <v>Euribor3MLastFixing_Quote</v>
+      </c>
+      <c r="L9" s="93"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D10" s="45" t="str">
@@ -10020,14 +9856,13 @@
         <v>41890</v>
       </c>
       <c r="I10" s="37">
-        <v>3.8848394143480331E-3</v>
-      </c>
-      <c r="K10" s="92" t="s">
-        <v>107</v>
-      </c>
-      <c r="L10" s="93">
-        <v>3.003E-3</v>
-      </c>
+        <v>3.8837608133420664E-3</v>
+      </c>
+      <c r="K10" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D10,Trigger)</f>
+        <v>Euribor6MLastFixing_Quote</v>
+      </c>
+      <c r="L10" s="93"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D11" s="45" t="str">
@@ -10050,52 +9885,50 @@
         <v>41981</v>
       </c>
       <c r="I11" s="37">
-        <v>4.7238193010242348E-3</v>
-      </c>
-      <c r="K11" s="92" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11" s="93" t="e">
-        <v>#NUM!</v>
-      </c>
+        <v>4.7230925017797392E-3</v>
+      </c>
+      <c r="K11" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D11,Trigger)</f>
+        <v>Euribor9MLastFixing_Quote</v>
+      </c>
+      <c r="L11" s="93"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D12" s="45" t="str">
-        <v>EUR_YCSTDRH_1YD</v>
+        <v>EUR_YCSTDRH_FUT3MU4</v>
       </c>
       <c r="E12" s="44">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>5.5200000000000006E-3</v>
-      </c>
-      <c r="F12" s="44" t="str">
+        <v>2.475000000000005E-3</v>
+      </c>
+      <c r="F12" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G12" s="43">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41704</v>
+        <v>41899</v>
       </c>
       <c r="H12" s="42">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>42069</v>
+        <v>41990</v>
       </c>
       <c r="I12" s="37">
-        <v>5.5592131683243132E-3</v>
-      </c>
-      <c r="K12" s="92" t="s">
-        <v>109</v>
-      </c>
-      <c r="L12" s="93" t="e">
-        <v>#NUM!</v>
-      </c>
+        <v>3.5060268614436701E-3</v>
+      </c>
+      <c r="K12" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D12,Trigger)</f>
+        <v>EURFUT3MU4_Quote</v>
+      </c>
+      <c r="L12" s="93"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D13" s="45" t="str">
-        <v>EUR_YCSTDRH_FUT3MH5</v>
+        <v>EUR_YCSTDRH_FUT3MZ4</v>
       </c>
       <c r="E13" s="44">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>3.0250000000000554E-3</v>
+        <v>2.6749999999999829E-3</v>
       </c>
       <c r="F13" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10103,29 +9936,28 @@
       </c>
       <c r="G13" s="43">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42081</v>
+        <v>41990</v>
       </c>
       <c r="H13" s="42">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>42173</v>
+        <v>42080</v>
       </c>
       <c r="I13" s="37">
-        <v>5.0223354206880358E-3</v>
-      </c>
-      <c r="K13" s="92" t="s">
-        <v>110</v>
-      </c>
-      <c r="L13" s="93">
-        <v>4.0689999999999997E-3</v>
-      </c>
+        <v>3.3167933959241092E-3</v>
+      </c>
+      <c r="K13" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D13,Trigger)</f>
+        <v>EURFUT3MZ4_Quote</v>
+      </c>
+      <c r="L13" s="93"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D14" s="45" t="str">
-        <v>EUR_YCSTDRH_FUT3MM5</v>
+        <v>EUR_YCSTDRH_FUT3MH5</v>
       </c>
       <c r="E14" s="44">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>3.4250000000000114E-3</v>
+        <v>2.9749999999999499E-3</v>
       </c>
       <c r="F14" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -10133,29 +9965,28 @@
       </c>
       <c r="G14" s="43">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>42172</v>
+        <v>42081</v>
       </c>
       <c r="H14" s="42">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42264</v>
+        <v>42173</v>
       </c>
       <c r="I14" s="37">
-        <v>4.7727056535376792E-3</v>
-      </c>
-      <c r="K14" s="92" t="s">
-        <v>111</v>
-      </c>
-      <c r="L14" s="93" t="e">
-        <v>#NUM!</v>
-      </c>
+        <v>3.2573640331369702E-3</v>
+      </c>
+      <c r="K14" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D14,Trigger)</f>
+        <v>EURFUT3MH5_Quote</v>
+      </c>
+      <c r="L14" s="93"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D15" s="45" t="str">
-        <v>EUR_YCSTDRH_FUT3MU5</v>
+        <v>EUR_YCSTDRH_FUT3MM5</v>
       </c>
       <c r="E15" s="44">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>3.9750000000000618E-3</v>
+        <v>3.3750000000000169E-3</v>
       </c>
       <c r="F15" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -10163,29 +9994,28 @@
       </c>
       <c r="G15" s="43">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>42263</v>
+        <v>42172</v>
       </c>
       <c r="H15" s="42">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42354</v>
+        <v>42264</v>
       </c>
       <c r="I15" s="37">
-        <v>4.6711528014068051E-3</v>
-      </c>
-      <c r="K15" s="92" t="s">
-        <v>112</v>
-      </c>
-      <c r="L15" s="93" t="e">
-        <v>#NUM!</v>
-      </c>
+        <v>3.2845876380616411E-3</v>
+      </c>
+      <c r="K15" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D15,Trigger)</f>
+        <v>EURFUT3MM5_Quote</v>
+      </c>
+      <c r="L15" s="93"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="45" t="str">
-        <v>EUR_YCSTDRH_FUT3MZ5</v>
+        <v>EUR_YCSTDRH_FUT3MU5</v>
       </c>
       <c r="E16" s="44">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>4.7249999999999792E-3</v>
+        <v>3.9249999999999563E-3</v>
       </c>
       <c r="F16" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -10193,29 +10023,28 @@
       </c>
       <c r="G16" s="43">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>42354</v>
+        <v>42263</v>
       </c>
       <c r="H16" s="42">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>42445</v>
+        <v>42354</v>
       </c>
       <c r="I16" s="37">
-        <v>4.685435217502921E-3</v>
-      </c>
-      <c r="K16" s="92" t="s">
-        <v>196</v>
-      </c>
-      <c r="L16" s="93">
-        <v>2.9750000000000002E-3</v>
-      </c>
+        <v>3.3810461219112371E-3</v>
+      </c>
+      <c r="K16" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D16,Trigger)</f>
+        <v>EURFUT3MU5_Quote</v>
+      </c>
+      <c r="L16" s="93"/>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D17" s="45" t="str">
-        <v>EUR_YCSTDRH_FUT3MH6</v>
+        <v>EUR_YCSTDRH_FUT3MZ5</v>
       </c>
       <c r="E17" s="44">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>5.6249999999999911E-3</v>
+        <v>4.6250000000001013E-3</v>
       </c>
       <c r="F17" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -10223,29 +10052,28 @@
       </c>
       <c r="G17" s="43">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>42445</v>
+        <v>42354</v>
       </c>
       <c r="H17" s="42">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42537</v>
+        <v>42445</v>
       </c>
       <c r="I17" s="37">
-        <v>4.7971127047673132E-3</v>
-      </c>
-      <c r="K17" s="92" t="s">
-        <v>197</v>
-      </c>
-      <c r="L17" s="93">
-        <v>3.1749999999999999E-3</v>
-      </c>
+        <v>3.5409331263807223E-3</v>
+      </c>
+      <c r="K17" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D17,Trigger)</f>
+        <v>EURFUT3MZ5_Quote</v>
+      </c>
+      <c r="L17" s="93"/>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D18" s="45" t="str">
-        <v>EUR_YCSTDRH_FUT3MM6</v>
+        <v>EUR_YCSTDRH_AB6E3Y</v>
       </c>
       <c r="E18" s="44">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>6.724999999999981E-3</v>
+        <v>5.8899999999999994E-3</v>
       </c>
       <c r="F18" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -10253,29 +10081,28 @@
       </c>
       <c r="G18" s="43">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>42536</v>
+        <v>41704</v>
       </c>
       <c r="H18" s="42">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42628</v>
+        <v>42800</v>
       </c>
       <c r="I18" s="37">
-        <v>4.9962572905238806E-3</v>
-      </c>
-      <c r="K18" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="L18" s="93">
-        <v>3.5750000000000001E-3</v>
-      </c>
+        <v>5.873540704402885E-3</v>
+      </c>
+      <c r="K18" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D18,Trigger)</f>
+        <v>EURAB6E3Y_Quote</v>
+      </c>
+      <c r="L18" s="93"/>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D19" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E3Y</v>
+        <v>EUR_YCSTDRH_AB6E4Y</v>
       </c>
       <c r="E19" s="44">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>5.9699999999999996E-3</v>
+        <v>7.8100000000000001E-3</v>
       </c>
       <c r="F19" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -10287,25 +10114,24 @@
       </c>
       <c r="H19" s="42">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42800</v>
+        <v>43165</v>
       </c>
       <c r="I19" s="37">
-        <v>5.9445926531756241E-3</v>
-      </c>
-      <c r="K19" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="L19" s="93">
-        <v>4.1250000000000002E-3</v>
-      </c>
+        <v>7.8023784104798511E-3</v>
+      </c>
+      <c r="K19" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D19,Trigger)</f>
+        <v>EURAB6E4Y_Quote</v>
+      </c>
+      <c r="L19" s="93"/>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D20" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E4Y</v>
+        <v>EUR_YCSTDRH_AB6E5Y</v>
       </c>
       <c r="E20" s="44">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>7.9000000000000008E-3</v>
+        <v>9.8399999999999998E-3</v>
       </c>
       <c r="F20" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -10317,25 +10143,24 @@
       </c>
       <c r="H20" s="42">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>43165</v>
+        <v>43530</v>
       </c>
       <c r="I20" s="37">
-        <v>7.8835458073082364E-3</v>
-      </c>
-      <c r="K20" s="92" t="s">
-        <v>115</v>
-      </c>
-      <c r="L20" s="93">
-        <v>4.9249999999999997E-3</v>
-      </c>
+        <v>9.8547671957100961E-3</v>
+      </c>
+      <c r="K20" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D20,Trigger)</f>
+        <v>EURAB6E5Y_Quote</v>
+      </c>
+      <c r="L20" s="93"/>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D21" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E5Y</v>
+        <v>EUR_YCSTDRH_AB6E6Y</v>
       </c>
       <c r="E21" s="44">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>9.9299999999999996E-3</v>
+        <v>1.183E-2</v>
       </c>
       <c r="F21" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -10347,25 +10172,24 @@
       </c>
       <c r="H21" s="42">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>43530</v>
+        <v>43896</v>
       </c>
       <c r="I21" s="37">
-        <v>9.9359270181713887E-3</v>
-      </c>
-      <c r="K21" s="92" t="s">
-        <v>116</v>
-      </c>
-      <c r="L21" s="93">
-        <v>5.875E-3</v>
-      </c>
+        <v>1.1877990058397875E-2</v>
+      </c>
+      <c r="K21" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D21,Trigger)</f>
+        <v>EURAB6E6Y_Quote</v>
+      </c>
+      <c r="L21" s="93"/>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D22" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E6Y</v>
+        <v>EUR_YCSTDRH_AB6E7Y</v>
       </c>
       <c r="E22" s="44">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.191E-2</v>
+        <v>1.37E-2</v>
       </c>
       <c r="F22" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -10377,25 +10201,24 @@
       </c>
       <c r="H22" s="42">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>43896</v>
+        <v>44263</v>
       </c>
       <c r="I22" s="37">
-        <v>1.1948912447757387E-2</v>
-      </c>
-      <c r="K22" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="L22" s="93">
-        <v>6.6E-3</v>
-      </c>
+        <v>1.3802805701039637E-2</v>
+      </c>
+      <c r="K22" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D22,Trigger)</f>
+        <v>EURAB6E7Y_Quote</v>
+      </c>
+      <c r="L22" s="93"/>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D23" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E7Y</v>
+        <v>EUR_YCSTDRH_AB6E8Y</v>
       </c>
       <c r="E23" s="44">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.376E-2</v>
+        <v>1.541E-2</v>
       </c>
       <c r="F23" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -10407,25 +10230,24 @@
       </c>
       <c r="H23" s="42">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>44263</v>
+        <v>44627</v>
       </c>
       <c r="I23" s="37">
-        <v>1.3853041633344653E-2</v>
-      </c>
-      <c r="K23" s="92" t="s">
-        <v>118</v>
-      </c>
-      <c r="L23" s="93">
-        <v>8.8699999999999994E-3</v>
-      </c>
+        <v>1.5582046576123986E-2</v>
+      </c>
+      <c r="K23" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D23,Trigger)</f>
+        <v>EURAB6E8Y_Quote</v>
+      </c>
+      <c r="L23" s="93"/>
     </row>
     <row r="24" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D24" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E8Y</v>
+        <v>EUR_YCSTDRH_AB6E9Y</v>
       </c>
       <c r="E24" s="44">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.5449999999999998E-2</v>
+        <v>1.695E-2</v>
       </c>
       <c r="F24" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -10437,25 +10259,24 @@
       </c>
       <c r="H24" s="42">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>44627</v>
+        <v>44991</v>
       </c>
       <c r="I24" s="37">
-        <v>1.5611279681155938E-2</v>
-      </c>
-      <c r="K24" s="92" t="s">
-        <v>119</v>
-      </c>
-      <c r="L24" s="93">
-        <v>1.12E-2</v>
-      </c>
+        <v>1.720251322830655E-2</v>
+      </c>
+      <c r="K24" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D24,Trigger)</f>
+        <v>EURAB6E9Y_Quote</v>
+      </c>
+      <c r="L24" s="93"/>
     </row>
     <row r="25" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D25" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E9Y</v>
+        <v>EUR_YCSTDRH_AB6E10Y</v>
       </c>
       <c r="E25" s="44">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>1.6969999999999999E-2</v>
+        <v>1.8319999999999999E-2</v>
       </c>
       <c r="F25" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -10467,25 +10288,24 @@
       </c>
       <c r="H25" s="42">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>44991</v>
+        <v>45357</v>
       </c>
       <c r="I25" s="37">
-        <v>1.7210386987978051E-2</v>
-      </c>
-      <c r="K25" s="92" t="s">
-        <v>120</v>
-      </c>
-      <c r="L25" s="93">
-        <v>1.3390000000000001E-2</v>
-      </c>
+        <v>1.8655386197592331E-2</v>
+      </c>
+      <c r="K25" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D25,Trigger)</f>
+        <v>EURAB6E10Y_Quote</v>
+      </c>
+      <c r="L25" s="93"/>
     </row>
     <row r="26" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D26" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E10Y</v>
+        <v>EUR_YCSTDRH_AB6E11Y</v>
       </c>
       <c r="E26" s="44">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>1.8340000000000002E-2</v>
+        <v>1.951E-2</v>
       </c>
       <c r="F26" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -10497,25 +10317,24 @@
       </c>
       <c r="H26" s="42">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>45357</v>
+        <v>45722</v>
       </c>
       <c r="I26" s="37">
-        <v>1.866348779664119E-2</v>
-      </c>
-      <c r="K26" s="92" t="s">
-        <v>121</v>
-      </c>
-      <c r="L26" s="93">
-        <v>1.5389999999999999E-2</v>
-      </c>
+        <v>1.9935407326967098E-2</v>
+      </c>
+      <c r="K26" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D26,Trigger)</f>
+        <v>EURAB6E11Y_Quote</v>
+      </c>
+      <c r="L26" s="93"/>
     </row>
     <row r="27" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D27" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E11Y</v>
+        <v>EUR_YCSTDRH_AB6E12Y</v>
       </c>
       <c r="E27" s="44">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>1.9530000000000002E-2</v>
+        <v>2.0539999999999999E-2</v>
       </c>
       <c r="F27" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -10527,25 +10346,24 @@
       </c>
       <c r="H27" s="42">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>45722</v>
+        <v>46087</v>
       </c>
       <c r="I27" s="37">
-        <v>1.9943795580953959E-2</v>
-      </c>
-      <c r="K27" s="92" t="s">
-        <v>122</v>
-      </c>
-      <c r="L27" s="93">
-        <v>1.719E-2</v>
-      </c>
+        <v>2.1054393930945912E-2</v>
+      </c>
+      <c r="K27" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D27,Trigger)</f>
+        <v>EURAB6E12Y_Quote</v>
+      </c>
+      <c r="L27" s="93"/>
     </row>
     <row r="28" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D28" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E12Y</v>
+        <v>EUR_YCSTDRH_AB6E13Y</v>
       </c>
       <c r="E28" s="44">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.0539999999999999E-2</v>
+        <v>2.1419999999999998E-2</v>
       </c>
       <c r="F28" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -10557,25 +10375,24 @@
       </c>
       <c r="H28" s="42">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>46087</v>
+        <v>46454</v>
       </c>
       <c r="I28" s="37">
-        <v>2.1040262784492395E-2</v>
-      </c>
-      <c r="K28" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="L28" s="93">
-        <v>1.8790000000000001E-2</v>
-      </c>
+        <v>2.2018153592467466E-2</v>
+      </c>
+      <c r="K28" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D28,Trigger)</f>
+        <v>EURAB6E13Y_Quote</v>
+      </c>
+      <c r="L28" s="93"/>
     </row>
     <row r="29" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D29" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E13Y</v>
+        <v>EUR_YCSTDRH_AB6E14Y</v>
       </c>
       <c r="E29" s="44">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.1419999999999998E-2</v>
+        <v>2.2170000000000002E-2</v>
       </c>
       <c r="F29" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -10587,25 +10404,24 @@
       </c>
       <c r="H29" s="42">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>46454</v>
+        <v>46818</v>
       </c>
       <c r="I29" s="37">
-        <v>2.2004383054411283E-2</v>
-      </c>
-      <c r="K29" s="92" t="s">
-        <v>124</v>
-      </c>
-      <c r="L29" s="93">
-        <v>2.0199999999999999E-2</v>
-      </c>
+        <v>2.2841526125830614E-2</v>
+      </c>
+      <c r="K29" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D29,Trigger)</f>
+        <v>EURAB6E14Y_Quote</v>
+      </c>
+      <c r="L29" s="93"/>
     </row>
     <row r="30" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D30" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E14Y</v>
+        <v>EUR_YCSTDRH_AB6E15Y</v>
       </c>
       <c r="E30" s="44">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>2.2160000000000003E-2</v>
+        <v>2.2770000000000002E-2</v>
       </c>
       <c r="F30" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -10617,25 +10433,24 @@
       </c>
       <c r="H30" s="42">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>46818</v>
+        <v>47183</v>
       </c>
       <c r="I30" s="37">
-        <v>2.2816258111804689E-2</v>
-      </c>
-      <c r="K30" s="92" t="s">
-        <v>125</v>
-      </c>
-      <c r="L30" s="93">
-        <v>2.1420000000000002E-2</v>
-      </c>
+        <v>2.3503306694225977E-2</v>
+      </c>
+      <c r="K30" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D30,Trigger)</f>
+        <v>EURAB6E15Y_Quote</v>
+      </c>
+      <c r="L30" s="93"/>
     </row>
     <row r="31" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D31" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E15Y</v>
+        <v>EUR_YCSTDRH_AB6E16Y</v>
       </c>
       <c r="E31" s="44">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>2.2759999999999999E-2</v>
+        <v>2.3250000000000003E-2</v>
       </c>
       <c r="F31" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -10647,25 +10462,24 @@
       </c>
       <c r="H31" s="42">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>47183</v>
+        <v>47548</v>
       </c>
       <c r="I31" s="37">
-        <v>2.3478490444144171E-2</v>
-      </c>
-      <c r="K31" s="92" t="s">
-        <v>126</v>
-      </c>
-      <c r="L31" s="93">
-        <v>2.247E-2</v>
-      </c>
+        <v>2.4030413948602815E-2</v>
+      </c>
+      <c r="K31" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D31,Trigger)</f>
+        <v>EURAB6E16Y_Quote</v>
+      </c>
+      <c r="L31" s="93"/>
     </row>
     <row r="32" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D32" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E16Y</v>
+        <v>EUR_YCSTDRH_AB6E17Y</v>
       </c>
       <c r="E32" s="44">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>2.3239999999999997E-2</v>
+        <v>2.3629999999999998E-2</v>
       </c>
       <c r="F32" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -10677,25 +10491,24 @@
       </c>
       <c r="H32" s="42">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>47548</v>
+        <v>47913</v>
       </c>
       <c r="I32" s="37">
-        <v>2.4006078329953797E-2</v>
-      </c>
-      <c r="K32" s="92" t="s">
-        <v>127</v>
-      </c>
-      <c r="L32" s="93">
-        <v>2.3359999999999999E-2</v>
-      </c>
+        <v>2.4443349014147759E-2</v>
+      </c>
+      <c r="K32" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D32,Trigger)</f>
+        <v>EURAB6E17Y_Quote</v>
+      </c>
+      <c r="L32" s="93"/>
     </row>
     <row r="33" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D33" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E17Y</v>
+        <v>EUR_YCSTDRH_AB6E18Y</v>
       </c>
       <c r="E33" s="44">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>2.3620000000000002E-2</v>
+        <v>2.3929999999999996E-2</v>
       </c>
       <c r="F33" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -10707,25 +10520,24 @@
       </c>
       <c r="H33" s="42">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>47913</v>
+        <v>48281</v>
       </c>
       <c r="I33" s="37">
-        <v>2.441950964447033E-2</v>
-      </c>
-      <c r="K33" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="L33" s="93">
-        <v>2.41E-2</v>
-      </c>
+        <v>2.475977587807518E-2</v>
+      </c>
+      <c r="K33" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D33,Trigger)</f>
+        <v>EURAB6E18Y_Quote</v>
+      </c>
+      <c r="L33" s="93"/>
     </row>
     <row r="34" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D34" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E18Y</v>
+        <v>EUR_YCSTDRH_AB6E19Y</v>
       </c>
       <c r="E34" s="44">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.392E-2</v>
+        <v>2.4150000000000001E-2</v>
       </c>
       <c r="F34" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -10737,25 +10549,24 @@
       </c>
       <c r="H34" s="42">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>48281</v>
+        <v>48645</v>
       </c>
       <c r="I34" s="37">
-        <v>2.4736443376360665E-2</v>
-      </c>
-      <c r="K34" s="92" t="s">
-        <v>129</v>
-      </c>
-      <c r="L34" s="93">
-        <v>2.47E-2</v>
-      </c>
+        <v>2.4985314711422818E-2</v>
+      </c>
+      <c r="K34" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D34,Trigger)</f>
+        <v>EURAB6E19Y_Quote</v>
+      </c>
+      <c r="L34" s="93"/>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D35" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E19Y</v>
+        <v>EUR_YCSTDRH_AB6E20Y</v>
       </c>
       <c r="E35" s="44">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.4140000000000002E-2</v>
+        <v>2.4319999999999998E-2</v>
       </c>
       <c r="F35" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -10767,25 +10578,24 @@
       </c>
       <c r="H35" s="42">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>48645</v>
+        <v>49009</v>
       </c>
       <c r="I35" s="37">
-        <v>2.4962488049172001E-2</v>
-      </c>
-      <c r="K35" s="92" t="s">
-        <v>130</v>
-      </c>
-      <c r="L35" s="93">
-        <v>2.5180000000000001E-2</v>
-      </c>
+        <v>2.5152071164456054E-2</v>
+      </c>
+      <c r="K35" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D35,Trigger)</f>
+        <v>EURAB6E20Y_Quote</v>
+      </c>
+      <c r="L35" s="93"/>
     </row>
     <row r="36" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D36" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E20Y</v>
+        <v>EUR_YCSTDRH_AB6E21Y</v>
       </c>
       <c r="E36" s="44">
         <f>_xll.qlRateHelperRate($D36)</f>
-        <v>2.4310000000000002E-2</v>
+        <v>2.4460000000000003E-2</v>
       </c>
       <c r="F36" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
@@ -10797,25 +10607,24 @@
       </c>
       <c r="H36" s="42">
         <f>_xll.qlRateHelperLatestDate($D36)</f>
-        <v>49009</v>
+        <v>49374</v>
       </c>
       <c r="I36" s="37">
-        <v>2.5129737288429807E-2</v>
-      </c>
-      <c r="K36" s="92" t="s">
-        <v>131</v>
-      </c>
-      <c r="L36" s="93">
-        <v>2.555E-2</v>
-      </c>
+        <v>2.5284737213136128E-2</v>
+      </c>
+      <c r="K36" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D36,Trigger)</f>
+        <v>EURAB6E21Y_Quote</v>
+      </c>
+      <c r="L36" s="93"/>
     </row>
     <row r="37" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D37" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E21Y</v>
+        <v>EUR_YCSTDRH_AB6E22Y</v>
       </c>
       <c r="E37" s="44">
         <f>_xll.qlRateHelperRate($D37)</f>
-        <v>2.445E-2</v>
+        <v>2.4580000000000001E-2</v>
       </c>
       <c r="F37" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D37)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D37)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D37)),_xll.qlSwapRateHelperSpread($D37))</f>
@@ -10827,25 +10636,24 @@
       </c>
       <c r="H37" s="42">
         <f>_xll.qlRateHelperLatestDate($D37)</f>
-        <v>49374</v>
+        <v>49740</v>
       </c>
       <c r="I37" s="37">
-        <v>2.5262871848518831E-2</v>
-      </c>
-      <c r="K37" s="92" t="s">
-        <v>132</v>
-      </c>
-      <c r="L37" s="93">
-        <v>2.5829999999999999E-2</v>
-      </c>
+        <v>2.5392619901379466E-2</v>
+      </c>
+      <c r="K37" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D37,Trigger)</f>
+        <v>EURAB6E22Y_Quote</v>
+      </c>
+      <c r="L37" s="93"/>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D38" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E22Y</v>
+        <v>EUR_YCSTDRH_AB6E23Y</v>
       </c>
       <c r="E38" s="44">
         <f>_xll.qlRateHelperRate($D38)</f>
-        <v>2.4569999999999998E-2</v>
+        <v>2.4660000000000001E-2</v>
       </c>
       <c r="F38" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D38)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D38)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D38)),_xll.qlSwapRateHelperSpread($D38))</f>
@@ -10857,25 +10665,24 @@
       </c>
       <c r="H38" s="42">
         <f>_xll.qlRateHelperLatestDate($D38)</f>
-        <v>49740</v>
+        <v>50105</v>
       </c>
       <c r="I38" s="37">
-        <v>2.5371196031298057E-2</v>
-      </c>
-      <c r="K38" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="L38" s="93">
-        <v>2.605E-2</v>
-      </c>
+        <v>2.545385592805063E-2</v>
+      </c>
+      <c r="K38" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D38,Trigger)</f>
+        <v>EURAB6E23Y_Quote</v>
+      </c>
+      <c r="L38" s="93"/>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D39" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E23Y</v>
+        <v>EUR_YCSTDRH_AB6E24Y</v>
       </c>
       <c r="E39" s="44">
         <f>_xll.qlRateHelperRate($D39)</f>
-        <v>2.4649999999999998E-2</v>
+        <v>2.4729999999999999E-2</v>
       </c>
       <c r="F39" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D39)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D39)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D39)),_xll.qlSwapRateHelperSpread($D39))</f>
@@ -10887,25 +10694,24 @@
       </c>
       <c r="H39" s="42">
         <f>_xll.qlRateHelperLatestDate($D39)</f>
-        <v>50105</v>
+        <v>50472</v>
       </c>
       <c r="I39" s="37">
-        <v>2.5432864827003882E-2</v>
-      </c>
-      <c r="K39" s="92" t="s">
-        <v>134</v>
-      </c>
-      <c r="L39" s="93">
-        <v>2.6210000000000001E-2</v>
-      </c>
+        <v>2.5505220818465828E-2</v>
+      </c>
+      <c r="K39" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D39,Trigger)</f>
+        <v>EURAB6E24Y_Quote</v>
+      </c>
+      <c r="L39" s="93"/>
     </row>
     <row r="40" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D40" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E24Y</v>
+        <v>EUR_YCSTDRH_AB6E25Y</v>
       </c>
       <c r="E40" s="44">
         <f>_xll.qlRateHelperRate($D40)</f>
-        <v>2.4719999999999999E-2</v>
+        <v>2.477E-2</v>
       </c>
       <c r="F40" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D40)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D40)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D40)),_xll.qlSwapRateHelperSpread($D40))</f>
@@ -10917,25 +10723,24 @@
       </c>
       <c r="H40" s="42">
         <f>_xll.qlRateHelperLatestDate($D40)</f>
-        <v>50472</v>
+        <v>50836</v>
       </c>
       <c r="I40" s="37">
-        <v>2.5484635110028769E-2</v>
-      </c>
-      <c r="K40" s="92" t="s">
-        <v>135</v>
-      </c>
-      <c r="L40" s="93">
-        <v>2.6349999999999998E-2</v>
-      </c>
+        <v>2.5518584090940159E-2</v>
+      </c>
+      <c r="K40" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D40,Trigger)</f>
+        <v>EURAB6E25Y_Quote</v>
+      </c>
+      <c r="L40" s="93"/>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D41" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E25Y</v>
+        <v>EUR_YCSTDRH_AB6E26Y</v>
       </c>
       <c r="E41" s="44">
         <f>_xll.qlRateHelperRate($D41)</f>
-        <v>2.4760000000000001E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="F41" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D41)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D41)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D41)),_xll.qlSwapRateHelperSpread($D41))</f>
@@ -10947,25 +10752,24 @@
       </c>
       <c r="H41" s="42">
         <f>_xll.qlRateHelperLatestDate($D41)</f>
-        <v>50836</v>
+        <v>51201</v>
       </c>
       <c r="I41" s="37">
-        <v>2.5498392834022512E-2</v>
-      </c>
-      <c r="K41" s="92" t="s">
-        <v>136</v>
-      </c>
-      <c r="L41" s="93">
-        <v>2.6440000000000002E-2</v>
-      </c>
+        <v>2.5518383122196123E-2</v>
+      </c>
+      <c r="K41" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D41,Trigger)</f>
+        <v>EURAB6E26Y_Quote</v>
+      </c>
+      <c r="L41" s="93"/>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D42" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E26Y</v>
+        <v>EUR_YCSTDRH_AB6E27Y</v>
       </c>
       <c r="E42" s="44">
         <f>_xll.qlRateHelperRate($D42)</f>
-        <v>2.479E-2</v>
+        <v>2.4809999999999999E-2</v>
       </c>
       <c r="F42" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D42)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D42)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D42)),_xll.qlSwapRateHelperSpread($D42))</f>
@@ -10977,25 +10781,24 @@
       </c>
       <c r="H42" s="42">
         <f>_xll.qlRateHelperLatestDate($D42)</f>
-        <v>51201</v>
+        <v>51566</v>
       </c>
       <c r="I42" s="37">
-        <v>2.5498565960176956E-2</v>
-      </c>
-      <c r="K42" s="92" t="s">
-        <v>137</v>
-      </c>
-      <c r="L42" s="93">
-        <v>2.6519999999999998E-2</v>
-      </c>
+        <v>2.5495036133639796E-2</v>
+      </c>
+      <c r="K42" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D42,Trigger)</f>
+        <v>EURAB6E27Y_Quote</v>
+      </c>
+      <c r="L42" s="93"/>
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D43" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E27Y</v>
+        <v>EUR_YCSTDRH_AB6E28Y</v>
       </c>
       <c r="E43" s="44">
         <f>_xll.qlRateHelperRate($D43)</f>
-        <v>2.4799999999999999E-2</v>
+        <v>2.4809999999999999E-2</v>
       </c>
       <c r="F43" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D43)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D43)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D43)),_xll.qlSwapRateHelperSpread($D43))</f>
@@ -11007,25 +10810,24 @@
       </c>
       <c r="H43" s="42">
         <f>_xll.qlRateHelperLatestDate($D43)</f>
-        <v>51566</v>
+        <v>51931</v>
       </c>
       <c r="I43" s="37">
-        <v>2.5475581897738492E-2</v>
-      </c>
-      <c r="K43" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="L43" s="93">
-        <v>2.657E-2</v>
-      </c>
+        <v>2.5459788367185793E-2</v>
+      </c>
+      <c r="K43" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D43,Trigger)</f>
+        <v>EURAB6E28Y_Quote</v>
+      </c>
+      <c r="L43" s="93"/>
     </row>
     <row r="44" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D44" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E28Y</v>
+        <v>EUR_YCSTDRH_AB6E29Y</v>
       </c>
       <c r="E44" s="44">
         <f>_xll.qlRateHelperRate($D44)</f>
-        <v>2.4809999999999999E-2</v>
+        <v>2.4820000000000002E-2</v>
       </c>
       <c r="F44" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D44)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D44)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D44)),_xll.qlSwapRateHelperSpread($D44))</f>
@@ -11037,25 +10839,24 @@
       </c>
       <c r="H44" s="42">
         <f>_xll.qlRateHelperLatestDate($D44)</f>
-        <v>51931</v>
+        <v>52296</v>
       </c>
       <c r="I44" s="37">
-        <v>2.5455284855313905E-2</v>
-      </c>
-      <c r="K44" s="92" t="s">
-        <v>139</v>
-      </c>
-      <c r="L44" s="93">
-        <v>2.6599999999999999E-2</v>
-      </c>
+        <v>2.5441766460900669E-2</v>
+      </c>
+      <c r="K44" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D44,Trigger)</f>
+        <v>EURAB6E29Y_Quote</v>
+      </c>
+      <c r="L44" s="93"/>
     </row>
     <row r="45" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D45" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E29Y</v>
+        <v>EUR_YCSTDRH_AB6E30Y</v>
       </c>
       <c r="E45" s="44">
         <f>_xll.qlRateHelperRate($D45)</f>
-        <v>2.4809999999999999E-2</v>
+        <v>2.4820000000000002E-2</v>
       </c>
       <c r="F45" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D45)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D45)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D45)),_xll.qlSwapRateHelperSpread($D45))</f>
@@ -11067,25 +10868,24 @@
       </c>
       <c r="H45" s="42">
         <f>_xll.qlRateHelperLatestDate($D45)</f>
-        <v>52296</v>
+        <v>52663</v>
       </c>
       <c r="I45" s="37">
-        <v>2.5422621065868119E-2</v>
-      </c>
-      <c r="K45" s="92" t="s">
-        <v>140</v>
-      </c>
-      <c r="L45" s="93">
-        <v>2.6610000000000002E-2</v>
-      </c>
+        <v>2.5408569357549898E-2</v>
+      </c>
+      <c r="K45" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D45,Trigger)</f>
+        <v>EURAB6E30Y_Quote</v>
+      </c>
+      <c r="L45" s="93"/>
     </row>
     <row r="46" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D46" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E30Y</v>
+        <v>EUR_YCSTDRH_AB6E35Y</v>
       </c>
       <c r="E46" s="44">
         <f>_xll.qlRateHelperRate($D46)</f>
-        <v>2.4809999999999999E-2</v>
+        <v>2.4910000000000002E-2</v>
       </c>
       <c r="F46" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D46)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D46)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D46)),_xll.qlSwapRateHelperSpread($D46))</f>
@@ -11097,25 +10897,24 @@
       </c>
       <c r="H46" s="42">
         <f>_xll.qlRateHelperLatestDate($D46)</f>
-        <v>52663</v>
+        <v>54490</v>
       </c>
       <c r="I46" s="37">
-        <v>2.5389739178924984E-2</v>
-      </c>
-      <c r="K46" s="92" t="s">
-        <v>141</v>
-      </c>
-      <c r="L46" s="93">
-        <v>2.6620000000000001E-2</v>
-      </c>
+        <v>2.5416534593185325E-2</v>
+      </c>
+      <c r="K46" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D46,Trigger)</f>
+        <v>EURAB6E35Y_Quote</v>
+      </c>
+      <c r="L46" s="93"/>
     </row>
     <row r="47" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D47" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E35Y</v>
+        <v>EUR_YCSTDRH_AB6E40Y</v>
       </c>
       <c r="E47" s="44">
         <f>_xll.qlRateHelperRate($D47)</f>
-        <v>2.4889999999999999E-2</v>
+        <v>2.5049999999999999E-2</v>
       </c>
       <c r="F47" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D47)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D47)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D47)),_xll.qlSwapRateHelperSpread($D47))</f>
@@ -11127,25 +10926,24 @@
       </c>
       <c r="H47" s="42">
         <f>_xll.qlRateHelperLatestDate($D47)</f>
-        <v>54490</v>
+        <v>56314</v>
       </c>
       <c r="I47" s="37">
-        <v>2.5383614965823184E-2</v>
-      </c>
-      <c r="K47" s="92" t="s">
-        <v>142</v>
-      </c>
-      <c r="L47" s="93">
-        <v>2.6610000000000002E-2</v>
-      </c>
+        <v>2.5543487884649101E-2</v>
+      </c>
+      <c r="K47" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D47,Trigger)</f>
+        <v>EURAB6E40Y_Quote</v>
+      </c>
+      <c r="L47" s="93"/>
     </row>
     <row r="48" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D48" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E40Y</v>
+        <v>EUR_YCSTDRH_AB6E50Y</v>
       </c>
       <c r="E48" s="44">
         <f>_xll.qlRateHelperRate($D48)</f>
-        <v>2.5019999999999997E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="F48" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D48)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D48)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D48)),_xll.qlSwapRateHelperSpread($D48))</f>
@@ -11157,25 +10955,24 @@
       </c>
       <c r="H48" s="42">
         <f>_xll.qlRateHelperLatestDate($D48)</f>
-        <v>56314</v>
+        <v>59967</v>
       </c>
       <c r="I48" s="37">
-        <v>2.5495502787395968E-2</v>
-      </c>
-      <c r="K48" s="92" t="s">
-        <v>143</v>
-      </c>
-      <c r="L48" s="93">
-        <v>2.6599999999999999E-2</v>
-      </c>
+        <v>2.5648202606178106E-2</v>
+      </c>
+      <c r="K48" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D48,Trigger)</f>
+        <v>EURAB6E50Y_Quote</v>
+      </c>
+      <c r="L48" s="93"/>
     </row>
     <row r="49" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D49" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E50Y</v>
+        <v>EUR_YCSTDRH_AB6E60Y</v>
       </c>
       <c r="E49" s="44">
         <f>_xll.qlRateHelperRate($D49)</f>
-        <v>2.5160000000000002E-2</v>
+        <v>2.5329999999999998E-2</v>
       </c>
       <c r="F49" s="44">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D49)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D49)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D49)),_xll.qlSwapRateHelperSpread($D49))</f>
@@ -11187,47 +10984,45 @@
       </c>
       <c r="H49" s="42">
         <f>_xll.qlRateHelperLatestDate($D49)</f>
-        <v>59967</v>
+        <v>63619</v>
       </c>
       <c r="I49" s="37">
-        <v>2.5585430253052446E-2</v>
-      </c>
-      <c r="K49" s="92" t="s">
-        <v>144</v>
-      </c>
-      <c r="L49" s="93">
-        <v>2.6599999999999999E-2</v>
-      </c>
+        <v>2.5793399729359772E-2</v>
+      </c>
+      <c r="K49" s="92" t="str">
+        <f>_xll.qlRateHelperQuoteName(D49,Trigger)</f>
+        <v>EURAB6E60Y_Quote</v>
+      </c>
+      <c r="L49" s="93"/>
     </row>
     <row r="50" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D50" s="45" t="str">
-        <v>EUR_YCSTDRH_AB6E60Y</v>
-      </c>
-      <c r="E50" s="44">
+      <c r="D50" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E50" s="44" t="e">
         <f>_xll.qlRateHelperRate($D50)</f>
-        <v>2.529E-2</v>
-      </c>
-      <c r="F50" s="44">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F50" s="44" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D50)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D50)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D50)),_xll.qlSwapRateHelperSpread($D50))</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="43">
+        <v>--</v>
+      </c>
+      <c r="G50" s="43" t="e">
         <f>_xll.qlRateHelperEarliestDate($D50)</f>
-        <v>41704</v>
-      </c>
-      <c r="H50" s="42">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H50" s="42" t="e">
         <f>_xll.qlRateHelperLatestDate($D50)</f>
-        <v>63619</v>
-      </c>
-      <c r="I50" s="37">
-        <v>2.5733868722344396E-2</v>
-      </c>
-      <c r="K50" s="92" t="s">
-        <v>145</v>
-      </c>
-      <c r="L50" s="93">
-        <v>2.6679999999999999E-2</v>
-      </c>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I50" s="37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K50" s="92" t="e">
+        <f>_xll.qlRateHelperQuoteName(D50,Trigger)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L50" s="93"/>
     </row>
     <row r="51" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D51" s="45" t="e">
@@ -11252,12 +11047,8 @@
       <c r="I51" s="37" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K51" s="92" t="s">
-        <v>146</v>
-      </c>
-      <c r="L51" s="93">
-        <v>2.6839999999999999E-2</v>
-      </c>
+      <c r="K51" s="92"/>
+      <c r="L51" s="93"/>
     </row>
     <row r="52" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D52" s="45" t="e">
@@ -11282,12 +11073,8 @@
       <c r="I52" s="37" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K52" s="92" t="s">
-        <v>147</v>
-      </c>
-      <c r="L52" s="93">
-        <v>2.7029999999999998E-2</v>
-      </c>
+      <c r="K52" s="92"/>
+      <c r="L52" s="93"/>
     </row>
     <row r="53" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D53" s="45" t="e">
@@ -11312,12 +11099,8 @@
       <c r="I53" s="37" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K53" s="92" t="s">
-        <v>148</v>
-      </c>
-      <c r="L53" s="93">
-        <v>2.716E-2</v>
-      </c>
+      <c r="K53" s="92"/>
+      <c r="L53" s="93"/>
     </row>
     <row r="54" spans="4:12" x14ac:dyDescent="0.2">
       <c r="D54" s="45" t="e">
@@ -13087,7 +12870,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 IV5 SR5 ACN5 AMJ5 AWF5 BGB5 BPX5 BZT5 CJP5 CTL5 DDH5 DND5 DWZ5 EGV5 EQR5 FAN5 FKJ5 FUF5 GEB5 GNX5 GXT5 HHP5 HRL5 IBH5 ILD5 IUZ5 JEV5 JOR5 JYN5 KIJ5 KSF5 LCB5 LLX5 LVT5 MFP5 MPL5 MZH5 NJD5 NSZ5 OCV5 OMR5 OWN5 PGJ5 PQF5 QAB5 QJX5 QTT5 RDP5 RNL5 RXH5 SHD5 SQZ5 TAV5 TKR5 TUN5 UEJ5 UOF5 UYB5 VHX5 VRT5 WBP5 WLL5 WVH5 B65541 IV65541 SR65541 ACN65541 AMJ65541 AWF65541 BGB65541 BPX65541 BZT65541 CJP65541 CTL65541 DDH65541 DND65541 DWZ65541 EGV65541 EQR65541 FAN65541 FKJ65541 FUF65541 GEB65541 GNX65541 GXT65541 HHP65541 HRL65541 IBH65541 ILD65541 IUZ65541 JEV65541 JOR65541 JYN65541 KIJ65541 KSF65541 LCB65541 LLX65541 LVT65541 MFP65541 MPL65541 MZH65541 NJD65541 NSZ65541 OCV65541 OMR65541 OWN65541 PGJ65541 PQF65541 QAB65541 QJX65541 QTT65541 RDP65541 RNL65541 RXH65541 SHD65541 SQZ65541 TAV65541 TKR65541 TUN65541 UEJ65541 UOF65541 UYB65541 VHX65541 VRT65541 WBP65541 WLL65541 WVH65541 B131077 IV131077 SR131077 ACN131077 AMJ131077 AWF131077 BGB131077 BPX131077 BZT131077 CJP131077 CTL131077 DDH131077 DND131077 DWZ131077 EGV131077 EQR131077 FAN131077 FKJ131077 FUF131077 GEB131077 GNX131077 GXT131077 HHP131077 HRL131077 IBH131077 ILD131077 IUZ131077 JEV131077 JOR131077 JYN131077 KIJ131077 KSF131077 LCB131077 LLX131077 LVT131077 MFP131077 MPL131077 MZH131077 NJD131077 NSZ131077 OCV131077 OMR131077 OWN131077 PGJ131077 PQF131077 QAB131077 QJX131077 QTT131077 RDP131077 RNL131077 RXH131077 SHD131077 SQZ131077 TAV131077 TKR131077 TUN131077 UEJ131077 UOF131077 UYB131077 VHX131077 VRT131077 WBP131077 WLL131077 WVH131077 B196613 IV196613 SR196613 ACN196613 AMJ196613 AWF196613 BGB196613 BPX196613 BZT196613 CJP196613 CTL196613 DDH196613 DND196613 DWZ196613 EGV196613 EQR196613 FAN196613 FKJ196613 FUF196613 GEB196613 GNX196613 GXT196613 HHP196613 HRL196613 IBH196613 ILD196613 IUZ196613 JEV196613 JOR196613 JYN196613 KIJ196613 KSF196613 LCB196613 LLX196613 LVT196613 MFP196613 MPL196613 MZH196613 NJD196613 NSZ196613 OCV196613 OMR196613 OWN196613 PGJ196613 PQF196613 QAB196613 QJX196613 QTT196613 RDP196613 RNL196613 RXH196613 SHD196613 SQZ196613 TAV196613 TKR196613 TUN196613 UEJ196613 UOF196613 UYB196613 VHX196613 VRT196613 WBP196613 WLL196613 WVH196613 B262149 IV262149 SR262149 ACN262149 AMJ262149 AWF262149 BGB262149 BPX262149 BZT262149 CJP262149 CTL262149 DDH262149 DND262149 DWZ262149 EGV262149 EQR262149 FAN262149 FKJ262149 FUF262149 GEB262149 GNX262149 GXT262149 HHP262149 HRL262149 IBH262149 ILD262149 IUZ262149 JEV262149 JOR262149 JYN262149 KIJ262149 KSF262149 LCB262149 LLX262149 LVT262149 MFP262149 MPL262149 MZH262149 NJD262149 NSZ262149 OCV262149 OMR262149 OWN262149 PGJ262149 PQF262149 QAB262149 QJX262149 QTT262149 RDP262149 RNL262149 RXH262149 SHD262149 SQZ262149 TAV262149 TKR262149 TUN262149 UEJ262149 UOF262149 UYB262149 VHX262149 VRT262149 WBP262149 WLL262149 WVH262149 B327685 IV327685 SR327685 ACN327685 AMJ327685 AWF327685 BGB327685 BPX327685 BZT327685 CJP327685 CTL327685 DDH327685 DND327685 DWZ327685 EGV327685 EQR327685 FAN327685 FKJ327685 FUF327685 GEB327685 GNX327685 GXT327685 HHP327685 HRL327685 IBH327685 ILD327685 IUZ327685 JEV327685 JOR327685 JYN327685 KIJ327685 KSF327685 LCB327685 LLX327685 LVT327685 MFP327685 MPL327685 MZH327685 NJD327685 NSZ327685 OCV327685 OMR327685 OWN327685 PGJ327685 PQF327685 QAB327685 QJX327685 QTT327685 RDP327685 RNL327685 RXH327685 SHD327685 SQZ327685 TAV327685 TKR327685 TUN327685 UEJ327685 UOF327685 UYB327685 VHX327685 VRT327685 WBP327685 WLL327685 WVH327685 B393221 IV393221 SR393221 ACN393221 AMJ393221 AWF393221 BGB393221 BPX393221 BZT393221 CJP393221 CTL393221 DDH393221 DND393221 DWZ393221 EGV393221 EQR393221 FAN393221 FKJ393221 FUF393221 GEB393221 GNX393221 GXT393221 HHP393221 HRL393221 IBH393221 ILD393221 IUZ393221 JEV393221 JOR393221 JYN393221 KIJ393221 KSF393221 LCB393221 LLX393221 LVT393221 MFP393221 MPL393221 MZH393221 NJD393221 NSZ393221 OCV393221 OMR393221 OWN393221 PGJ393221 PQF393221 QAB393221 QJX393221 QTT393221 RDP393221 RNL393221 RXH393221 SHD393221 SQZ393221 TAV393221 TKR393221 TUN393221 UEJ393221 UOF393221 UYB393221 VHX393221 VRT393221 WBP393221 WLL393221 WVH393221 B458757 IV458757 SR458757 ACN458757 AMJ458757 AWF458757 BGB458757 BPX458757 BZT458757 CJP458757 CTL458757 DDH458757 DND458757 DWZ458757 EGV458757 EQR458757 FAN458757 FKJ458757 FUF458757 GEB458757 GNX458757 GXT458757 HHP458757 HRL458757 IBH458757 ILD458757 IUZ458757 JEV458757 JOR458757 JYN458757 KIJ458757 KSF458757 LCB458757 LLX458757 LVT458757 MFP458757 MPL458757 MZH458757 NJD458757 NSZ458757 OCV458757 OMR458757 OWN458757 PGJ458757 PQF458757 QAB458757 QJX458757 QTT458757 RDP458757 RNL458757 RXH458757 SHD458757 SQZ458757 TAV458757 TKR458757 TUN458757 UEJ458757 UOF458757 UYB458757 VHX458757 VRT458757 WBP458757 WLL458757 WVH458757 B524293 IV524293 SR524293 ACN524293 AMJ524293 AWF524293 BGB524293 BPX524293 BZT524293 CJP524293 CTL524293 DDH524293 DND524293 DWZ524293 EGV524293 EQR524293 FAN524293 FKJ524293 FUF524293 GEB524293 GNX524293 GXT524293 HHP524293 HRL524293 IBH524293 ILD524293 IUZ524293 JEV524293 JOR524293 JYN524293 KIJ524293 KSF524293 LCB524293 LLX524293 LVT524293 MFP524293 MPL524293 MZH524293 NJD524293 NSZ524293 OCV524293 OMR524293 OWN524293 PGJ524293 PQF524293 QAB524293 QJX524293 QTT524293 RDP524293 RNL524293 RXH524293 SHD524293 SQZ524293 TAV524293 TKR524293 TUN524293 UEJ524293 UOF524293 UYB524293 VHX524293 VRT524293 WBP524293 WLL524293 WVH524293 B589829 IV589829 SR589829 ACN589829 AMJ589829 AWF589829 BGB589829 BPX589829 BZT589829 CJP589829 CTL589829 DDH589829 DND589829 DWZ589829 EGV589829 EQR589829 FAN589829 FKJ589829 FUF589829 GEB589829 GNX589829 GXT589829 HHP589829 HRL589829 IBH589829 ILD589829 IUZ589829 JEV589829 JOR589829 JYN589829 KIJ589829 KSF589829 LCB589829 LLX589829 LVT589829 MFP589829 MPL589829 MZH589829 NJD589829 NSZ589829 OCV589829 OMR589829 OWN589829 PGJ589829 PQF589829 QAB589829 QJX589829 QTT589829 RDP589829 RNL589829 RXH589829 SHD589829 SQZ589829 TAV589829 TKR589829 TUN589829 UEJ589829 UOF589829 UYB589829 VHX589829 VRT589829 WBP589829 WLL589829 WVH589829 B655365 IV655365 SR655365 ACN655365 AMJ655365 AWF655365 BGB655365 BPX655365 BZT655365 CJP655365 CTL655365 DDH655365 DND655365 DWZ655365 EGV655365 EQR655365 FAN655365 FKJ655365 FUF655365 GEB655365 GNX655365 GXT655365 HHP655365 HRL655365 IBH655365 ILD655365 IUZ655365 JEV655365 JOR655365 JYN655365 KIJ655365 KSF655365 LCB655365 LLX655365 LVT655365 MFP655365 MPL655365 MZH655365 NJD655365 NSZ655365 OCV655365 OMR655365 OWN655365 PGJ655365 PQF655365 QAB655365 QJX655365 QTT655365 RDP655365 RNL655365 RXH655365 SHD655365 SQZ655365 TAV655365 TKR655365 TUN655365 UEJ655365 UOF655365 UYB655365 VHX655365 VRT655365 WBP655365 WLL655365 WVH655365 B720901 IV720901 SR720901 ACN720901 AMJ720901 AWF720901 BGB720901 BPX720901 BZT720901 CJP720901 CTL720901 DDH720901 DND720901 DWZ720901 EGV720901 EQR720901 FAN720901 FKJ720901 FUF720901 GEB720901 GNX720901 GXT720901 HHP720901 HRL720901 IBH720901 ILD720901 IUZ720901 JEV720901 JOR720901 JYN720901 KIJ720901 KSF720901 LCB720901 LLX720901 LVT720901 MFP720901 MPL720901 MZH720901 NJD720901 NSZ720901 OCV720901 OMR720901 OWN720901 PGJ720901 PQF720901 QAB720901 QJX720901 QTT720901 RDP720901 RNL720901 RXH720901 SHD720901 SQZ720901 TAV720901 TKR720901 TUN720901 UEJ720901 UOF720901 UYB720901 VHX720901 VRT720901 WBP720901 WLL720901 WVH720901 B786437 IV786437 SR786437 ACN786437 AMJ786437 AWF786437 BGB786437 BPX786437 BZT786437 CJP786437 CTL786437 DDH786437 DND786437 DWZ786437 EGV786437 EQR786437 FAN786437 FKJ786437 FUF786437 GEB786437 GNX786437 GXT786437 HHP786437 HRL786437 IBH786437 ILD786437 IUZ786437 JEV786437 JOR786437 JYN786437 KIJ786437 KSF786437 LCB786437 LLX786437 LVT786437 MFP786437 MPL786437 MZH786437 NJD786437 NSZ786437 OCV786437 OMR786437 OWN786437 PGJ786437 PQF786437 QAB786437 QJX786437 QTT786437 RDP786437 RNL786437 RXH786437 SHD786437 SQZ786437 TAV786437 TKR786437 TUN786437 UEJ786437 UOF786437 UYB786437 VHX786437 VRT786437 WBP786437 WLL786437 WVH786437 B851973 IV851973 SR851973 ACN851973 AMJ851973 AWF851973 BGB851973 BPX851973 BZT851973 CJP851973 CTL851973 DDH851973 DND851973 DWZ851973 EGV851973 EQR851973 FAN851973 FKJ851973 FUF851973 GEB851973 GNX851973 GXT851973 HHP851973 HRL851973 IBH851973 ILD851973 IUZ851973 JEV851973 JOR851973 JYN851973 KIJ851973 KSF851973 LCB851973 LLX851973 LVT851973 MFP851973 MPL851973 MZH851973 NJD851973 NSZ851973 OCV851973 OMR851973 OWN851973 PGJ851973 PQF851973 QAB851973 QJX851973 QTT851973 RDP851973 RNL851973 RXH851973 SHD851973 SQZ851973 TAV851973 TKR851973 TUN851973 UEJ851973 UOF851973 UYB851973 VHX851973 VRT851973 WBP851973 WLL851973 WVH851973 B917509 IV917509 SR917509 ACN917509 AMJ917509 AWF917509 BGB917509 BPX917509 BZT917509 CJP917509 CTL917509 DDH917509 DND917509 DWZ917509 EGV917509 EQR917509 FAN917509 FKJ917509 FUF917509 GEB917509 GNX917509 GXT917509 HHP917509 HRL917509 IBH917509 ILD917509 IUZ917509 JEV917509 JOR917509 JYN917509 KIJ917509 KSF917509 LCB917509 LLX917509 LVT917509 MFP917509 MPL917509 MZH917509 NJD917509 NSZ917509 OCV917509 OMR917509 OWN917509 PGJ917509 PQF917509 QAB917509 QJX917509 QTT917509 RDP917509 RNL917509 RXH917509 SHD917509 SQZ917509 TAV917509 TKR917509 TUN917509 UEJ917509 UOF917509 UYB917509 VHX917509 VRT917509 WBP917509 WLL917509 WVH917509 B983045 IV983045 SR983045 ACN983045 AMJ983045 AWF983045 BGB983045 BPX983045 BZT983045 CJP983045 CTL983045 DDH983045 DND983045 DWZ983045 EGV983045 EQR983045 FAN983045 FKJ983045 FUF983045 GEB983045 GNX983045 GXT983045 HHP983045 HRL983045 IBH983045 ILD983045 IUZ983045 JEV983045 JOR983045 JYN983045 KIJ983045 KSF983045 LCB983045 LLX983045 LVT983045 MFP983045 MPL983045 MZH983045 NJD983045 NSZ983045 OCV983045 OMR983045 OWN983045 PGJ983045 PQF983045 QAB983045 QJX983045 QTT983045 RDP983045 RNL983045 RXH983045 SHD983045 SQZ983045 TAV983045 TKR983045 TUN983045 UEJ983045 UOF983045 UYB983045 VHX983045 VRT983045 WBP983045 WLL983045 WVH983045">
       <formula1>"AllDepos,DeposBeforeFirstFuturesStartDate,DeposBeforeFirstFuturesStartDatePlusOne,DeposBeforeFirstFuturesExpiryDate"</formula1>
     </dataValidation>
@@ -13105,7 +12888,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" activeCellId="6" sqref="A6:XFD6 A10:XFD10 A11:XFD11 A13:XFD13 A14:XFD14 A16:XFD16 A17:XFD17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -13123,12 +12906,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="118" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="B1" s="117"/>
       <c r="C1" s="117"/>
       <c r="D1" s="96" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="E1" s="116" t="str">
         <f>Currency&amp;"_YC"&amp;$D$1&amp;"RH"</f>
@@ -13142,10 +12925,10 @@
       <c r="A2" s="108"/>
       <c r="B2" s="115"/>
       <c r="C2" s="115" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="D2" s="115" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="E2" s="114" t="str">
         <f>$E$1&amp;"_Deposits.xml"</f>
@@ -13164,10 +12947,10 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="108"/>
       <c r="B3" s="111" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="C3" s="110" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="D3" s="105" t="str">
         <f>Currency&amp;$B3&amp;"D"&amp;QuoteSuffix</f>
@@ -13179,7 +12962,7 @@
       </c>
       <c r="F3" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_OND#0002</v>
+        <v>EUR_YCSTDRH_OND#0004</v>
       </c>
       <c r="G3" s="109" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13190,7 +12973,7 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="108"/>
       <c r="B4" s="107" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="C4" s="106" t="str">
         <f t="shared" ref="C4:C11" si="1">PROPER(Currency)&amp;FamilyName&amp;$B4</f>
@@ -13206,7 +12989,7 @@
       </c>
       <c r="F4" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_SWD#0002</v>
+        <v>EUR_YCSTDRH_SWD#0004</v>
       </c>
       <c r="G4" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13221,7 +13004,7 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="108"/>
       <c r="B5" s="107" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="C5" s="106" t="str">
         <f t="shared" si="1"/>
@@ -13237,7 +13020,7 @@
       </c>
       <c r="F5" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_2WD#0002</v>
+        <v>EUR_YCSTDRH_2WD#0004</v>
       </c>
       <c r="G5" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13248,7 +13031,7 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="108"/>
       <c r="B6" s="107" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="C6" s="106" t="str">
         <f t="shared" si="1"/>
@@ -13264,7 +13047,7 @@
       </c>
       <c r="F6" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_1MD#0002</v>
+        <v>EUR_YCSTDRH_1MD#0004</v>
       </c>
       <c r="G6" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13275,7 +13058,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="108"/>
       <c r="B7" s="107" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="C7" s="106" t="str">
         <f t="shared" si="1"/>
@@ -13291,7 +13074,7 @@
       </c>
       <c r="F7" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_2MD#0002</v>
+        <v>EUR_YCSTDRH_2MD#0004</v>
       </c>
       <c r="G7" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13302,7 +13085,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="108"/>
       <c r="B8" s="107" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="C8" s="106" t="str">
         <f t="shared" si="1"/>
@@ -13318,7 +13101,7 @@
       </c>
       <c r="F8" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_3MD#0003</v>
+        <v>EUR_YCSTDRH_3MD#0004</v>
       </c>
       <c r="G8" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13329,7 +13112,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="108"/>
       <c r="B9" s="107" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C9" s="106" t="str">
         <f t="shared" si="1"/>
@@ -13345,7 +13128,7 @@
       </c>
       <c r="F9" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_6MD#0002</v>
+        <v>EUR_YCSTDRH_6MD#0004</v>
       </c>
       <c r="G9" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13356,7 +13139,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="108"/>
       <c r="B10" s="107" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="C10" s="106" t="str">
         <f t="shared" si="1"/>
@@ -13372,7 +13155,7 @@
       </c>
       <c r="F10" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_9MD#0002</v>
+        <v>EUR_YCSTDRH_9MD#0004</v>
       </c>
       <c r="G10" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -13399,7 +13182,7 @@
       </c>
       <c r="F11" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_1YD#0002</v>
+        <v>EUR_YCSTDRH_1YD#0004</v>
       </c>
       <c r="G11" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -13448,13 +13231,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="166" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="B1" s="165"/>
       <c r="C1" s="165"/>
       <c r="D1" s="165"/>
       <c r="E1" s="164" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="G1" s="163" t="str">
         <f>Currency&amp;"_YC"&amp;$E$1&amp;"RH"</f>
@@ -13470,10 +13253,10 @@
       <c r="C2" s="159"/>
       <c r="D2" s="158"/>
       <c r="E2" s="157" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="F2" s="157" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="G2" s="156" t="str">
         <f>$G$1&amp;"_FRAs.xml"</f>
@@ -13492,16 +13275,16 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="149"/>
       <c r="B3" s="153" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="C3" s="153" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="D3" s="152" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="E3" s="151" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="F3" s="151" t="str">
         <f>Currency&amp;C3&amp;D3&amp;"_Quote"</f>
@@ -13513,7 +13296,7 @@
       </c>
       <c r="H3" s="151" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_TND#0001</v>
+        <v>EUR_YCSTDRH_TND#0004</v>
       </c>
       <c r="I3" s="150" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -13524,16 +13307,16 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="149"/>
       <c r="B4" s="148" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="C4" s="148" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="D4" s="147" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="E4" s="146" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="F4" s="146" t="str">
         <f>Currency&amp;C4&amp;D4&amp;"_Quote"</f>
@@ -13545,7 +13328,7 @@
       </c>
       <c r="H4" s="146" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_SND#0001</v>
+        <v>EUR_YCSTDRH_SND#0004</v>
       </c>
       <c r="I4" s="145" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -13602,13 +13385,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="184" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="B1" s="189"/>
       <c r="C1" s="189"/>
       <c r="D1" s="189"/>
       <c r="E1" s="188" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="F1" s="187"/>
       <c r="G1" s="187"/>
@@ -13623,22 +13406,22 @@
     <row r="2" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="184"/>
       <c r="B2" s="159" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="C2" s="157" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="D2" s="183" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E2" s="157" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="F2" s="157" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="G2" s="159" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="H2" s="156" t="str">
         <f>$H$1&amp;"_Futures"&amp;$E$1&amp;".xml"</f>
@@ -13684,7 +13467,7 @@
       </c>
       <c r="I3" s="179" t="str">
         <f>_xll.qlFuturesRateHelper(H3,$F3,$D3,$E3,$G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH4#0004</v>
       </c>
       <c r="J3" s="178" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -13722,7 +13505,7 @@
       </c>
       <c r="I4" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H4,$F4,$D4,$E4,$G4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MJ4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MJ4#0004</v>
       </c>
       <c r="J4" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -13760,7 +13543,7 @@
       </c>
       <c r="I5" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H5,$F5,$D5,$E5,$G5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MK4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MK4#0004</v>
       </c>
       <c r="J5" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13798,7 +13581,7 @@
       </c>
       <c r="I6" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H6,$F6,$D6,$E6,$G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM4#0004</v>
       </c>
       <c r="J6" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13836,7 +13619,7 @@
       </c>
       <c r="I7" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H7,$F7,$D7,$E7,$G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MN4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MN4#0004</v>
       </c>
       <c r="J7" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -13874,7 +13657,7 @@
       </c>
       <c r="I8" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H8,$F8,$D8,$E8,$G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MQ4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MQ4#0004</v>
       </c>
       <c r="J8" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -13912,7 +13695,7 @@
       </c>
       <c r="I9" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H9,$F9,$D9,$E9,$G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU4#0004</v>
       </c>
       <c r="J9" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -13950,7 +13733,7 @@
       </c>
       <c r="I10" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H10,$F10,$D10,$E10,$G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MV4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MV4#0004</v>
       </c>
       <c r="J10" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -13988,7 +13771,7 @@
       </c>
       <c r="I11" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H11,$F11,$D11,$E11,$G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MX4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MX4#0004</v>
       </c>
       <c r="J11" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -14026,7 +13809,7 @@
       </c>
       <c r="I12" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H12,$F12,$D12,$E12,$G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ4#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ4#0004</v>
       </c>
       <c r="J12" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -14064,7 +13847,7 @@
       </c>
       <c r="I13" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H13,$F13,$D13,$E13,$G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MF5#0001</v>
+        <v>EUR_YCSTDRH_FUT3MF5#0004</v>
       </c>
       <c r="J13" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -14102,7 +13885,7 @@
       </c>
       <c r="I14" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H14,$F14,$D14,$E14,$G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MG5#0001</v>
+        <v>EUR_YCSTDRH_FUT3MG5#0004</v>
       </c>
       <c r="J14" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -14140,7 +13923,7 @@
       </c>
       <c r="I15" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H15,$F15,$D15,$E15,$G15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH5#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH5#0004</v>
       </c>
       <c r="J15" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -14254,7 +14037,7 @@
       </c>
       <c r="I18" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H18,$F18,$D18,$E18,$G18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM5#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM5#0004</v>
       </c>
       <c r="J18" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -14368,7 +14151,7 @@
       </c>
       <c r="I21" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H21,$F21,$D21,$E21,$G21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU5#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU5#0004</v>
       </c>
       <c r="J21" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -14482,7 +14265,7 @@
       </c>
       <c r="I24" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H24,$F24,$D24,$E24,$G24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ5#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ5#0004</v>
       </c>
       <c r="J24" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -14596,7 +14379,7 @@
       </c>
       <c r="I27" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H27,$F27,$D27,$E27,$G27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH6#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH6#0004</v>
       </c>
       <c r="J27" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -14710,7 +14493,7 @@
       </c>
       <c r="I30" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H30,$F30,$D30,$E30,$G30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM6#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM6#0004</v>
       </c>
       <c r="J30" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -14824,7 +14607,7 @@
       </c>
       <c r="I33" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H33,$F33,$D33,$E33,$G33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU6#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU6#0004</v>
       </c>
       <c r="J33" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -14938,7 +14721,7 @@
       </c>
       <c r="I36" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H36,$F36,$D36,$E36,$G36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ6#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ6#0004</v>
       </c>
       <c r="J36" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -15052,7 +14835,7 @@
       </c>
       <c r="I39" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H39,$F39,$D39,$E39,$G39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH7#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH7#0004</v>
       </c>
       <c r="J39" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -15164,7 +14947,7 @@
       </c>
       <c r="I42" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H42,$F42,$D42,$E42,$G42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM7#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM7#0004</v>
       </c>
       <c r="J42" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -15275,7 +15058,7 @@
       </c>
       <c r="I45" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H45,$F45,$D45,$E45,$G45,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU7#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU7#0004</v>
       </c>
       <c r="J45" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I45)</f>
@@ -15386,7 +15169,7 @@
       </c>
       <c r="I48" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H48,$F48,$D48,$E48,$G48,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ7#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ7#0004</v>
       </c>
       <c r="J48" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I48)</f>
@@ -15497,7 +15280,7 @@
       </c>
       <c r="I51" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H51,$F51,$D51,$E51,$G51,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH8#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH8#0004</v>
       </c>
       <c r="J51" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I51)</f>
@@ -15608,7 +15391,7 @@
       </c>
       <c r="I54" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H54,$F54,$D54,$E54,$G54,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM8#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM8#0004</v>
       </c>
       <c r="J54" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I54)</f>
@@ -15719,7 +15502,7 @@
       </c>
       <c r="I57" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H57,$F57,$D57,$E57,$G57,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU8#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU8#0004</v>
       </c>
       <c r="J57" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I57)</f>
@@ -15830,7 +15613,7 @@
       </c>
       <c r="I60" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H60,$F60,$D60,$E60,$G60,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ8#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ8#0004</v>
       </c>
       <c r="J60" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I60)</f>
@@ -15941,7 +15724,7 @@
       </c>
       <c r="I63" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H63,$F63,$D63,$E63,$G63,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH9#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH9#0004</v>
       </c>
       <c r="J63" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I63)</f>
@@ -16052,7 +15835,7 @@
       </c>
       <c r="I66" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H66,$F66,$D66,$E66,$G66,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM9#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM9#0004</v>
       </c>
       <c r="J66" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I66)</f>
@@ -16163,7 +15946,7 @@
       </c>
       <c r="I69" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H69,$F69,$D69,$E69,$G69,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU9#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU9#0004</v>
       </c>
       <c r="J69" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I69)</f>
@@ -16274,7 +16057,7 @@
       </c>
       <c r="I72" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H72,$F72,$D72,$E72,$G72,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ9#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ9#0004</v>
       </c>
       <c r="J72" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I72)</f>
@@ -16385,7 +16168,7 @@
       </c>
       <c r="I75" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H75,$F75,$D75,$E75,$G75,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH0#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH0#0004</v>
       </c>
       <c r="J75" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I75)</f>
@@ -16496,7 +16279,7 @@
       </c>
       <c r="I78" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H78,$F78,$D78,$E78,$G78,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM0#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM0#0004</v>
       </c>
       <c r="J78" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I78)</f>
@@ -16607,7 +16390,7 @@
       </c>
       <c r="I81" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H81,$F81,$D81,$E81,$G81,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU0#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU0#0004</v>
       </c>
       <c r="J81" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I81)</f>
@@ -16718,7 +16501,7 @@
       </c>
       <c r="I84" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H84,$F84,$D84,$E84,$G84,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ0#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ0#0004</v>
       </c>
       <c r="J84" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I84)</f>
@@ -16829,7 +16612,7 @@
       </c>
       <c r="I87" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H87,$F87,$D87,$E87,$G87,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH1#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH1#0004</v>
       </c>
       <c r="J87" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I87)</f>
@@ -16940,7 +16723,7 @@
       </c>
       <c r="I90" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H90,$F90,$D90,$E90,$G90,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM1#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM1#0004</v>
       </c>
       <c r="J90" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I90)</f>
@@ -17051,7 +16834,7 @@
       </c>
       <c r="I93" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H93,$F93,$D93,$E93,$G93,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MU1#0001</v>
+        <v>EUR_YCSTDRH_FUT3MU1#0004</v>
       </c>
       <c r="J93" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I93)</f>
@@ -17162,7 +16945,7 @@
       </c>
       <c r="I96" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H96,$F96,$D96,$E96,$G96,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MZ1#0001</v>
+        <v>EUR_YCSTDRH_FUT3MZ1#0004</v>
       </c>
       <c r="J96" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I96)</f>
@@ -17273,7 +17056,7 @@
       </c>
       <c r="I99" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H99,$F99,$D99,$E99,$G99,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MH2#0001</v>
+        <v>EUR_YCSTDRH_FUT3MH2#0004</v>
       </c>
       <c r="J99" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I99)</f>
@@ -17384,7 +17167,7 @@
       </c>
       <c r="I102" s="171" t="str">
         <f>_xll.qlFuturesRateHelper(H102,$F102,$D102,$E102,$G102,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_FUT3MM2#0001</v>
+        <v>EUR_YCSTDRH_FUT3MM2#0004</v>
       </c>
       <c r="J102" s="170" t="str">
         <f>_xll.ohRangeRetrieveError(I102)</f>
@@ -18157,7 +17940,9 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18180,7 +17965,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="166" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B1" s="165"/>
       <c r="C1" s="165"/>
@@ -18207,7 +17992,7 @@
       <c r="H2" s="200"/>
       <c r="I2" s="200"/>
       <c r="J2" s="188" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="K2" s="188" t="str">
         <f>Currency&amp;"_YC"&amp;"STDRH"</f>
@@ -18223,25 +18008,25 @@
     <row r="3" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="149"/>
       <c r="B3" s="157" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="C3" s="157"/>
       <c r="D3" s="157"/>
       <c r="E3" s="157"/>
       <c r="F3" s="157" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="G3" s="157" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="H3" s="157" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="I3" s="157" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="J3" s="157" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="K3" s="205" t="str">
         <f>K2&amp;"_Swaps.xml"</f>
@@ -18274,7 +18059,7 @@
       </c>
       <c r="L4" s="203" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YCSTDRH_AB6E_ibor6M#0001</v>
+        <v>EUR_YCSTDRH_AB6E_ibor6M#0004</v>
       </c>
       <c r="M4" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -18301,7 +18086,7 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="149"/>
       <c r="B6" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C6" s="198" t="s">
         <v>36</v>
@@ -18317,7 +18102,7 @@
         <v>Annual</v>
       </c>
       <c r="G6" s="174" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H6" s="174" t="str">
         <f>IF(UPPER(RIGHT($D6))="B",BondBasisDayCounter,IF(UPPER(RIGHT($D6))="M",MoneyMarketDayCounter,"--"))</f>
@@ -18336,7 +18121,7 @@
       </c>
       <c r="L6" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E1Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E1Y#0004</v>
       </c>
       <c r="M6" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -18351,7 +18136,7 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="149"/>
       <c r="B7" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C7" s="198" t="s">
         <v>35</v>
@@ -18367,7 +18152,7 @@
         <v>Annual</v>
       </c>
       <c r="G7" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H7" s="173" t="str">
         <f t="shared" ref="H7:H42" si="3">IF(UPPER(RIGHT($D7))="B",BondBasisDayCounter,IF(UPPER(RIGHT($D7))="M",MoneyMarketDayCounter,"--"))</f>
@@ -18386,7 +18171,7 @@
       </c>
       <c r="L7" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E15M#0001</v>
+        <v>EUR_YCSTDRH_AB6E15M#0004</v>
       </c>
       <c r="M7" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -18397,7 +18182,7 @@
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="149"/>
       <c r="B8" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C8" s="198" t="s">
         <v>34</v>
@@ -18413,7 +18198,7 @@
         <v>Annual</v>
       </c>
       <c r="G8" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H8" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18432,7 +18217,7 @@
       </c>
       <c r="L8" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E18M#0001</v>
+        <v>EUR_YCSTDRH_AB6E18M#0004</v>
       </c>
       <c r="M8" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -18443,7 +18228,7 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="149"/>
       <c r="B9" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C9" s="198" t="s">
         <v>33</v>
@@ -18459,7 +18244,7 @@
         <v>Annual</v>
       </c>
       <c r="G9" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H9" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18478,7 +18263,7 @@
       </c>
       <c r="L9" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E21M#0001</v>
+        <v>EUR_YCSTDRH_AB6E21M#0004</v>
       </c>
       <c r="M9" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -18489,7 +18274,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="149"/>
       <c r="B10" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C10" s="198" t="s">
         <v>32</v>
@@ -18505,7 +18290,7 @@
         <v>Annual</v>
       </c>
       <c r="G10" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H10" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18524,7 +18309,7 @@
       </c>
       <c r="L10" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E2Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E2Y#0004</v>
       </c>
       <c r="M10" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -18535,7 +18320,7 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="149"/>
       <c r="B11" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C11" s="198" t="s">
         <v>31</v>
@@ -18551,7 +18336,7 @@
         <v>Annual</v>
       </c>
       <c r="G11" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H11" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18570,7 +18355,7 @@
       </c>
       <c r="L11" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E3Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E3Y#0004</v>
       </c>
       <c r="M11" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -18581,7 +18366,7 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="149"/>
       <c r="B12" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C12" s="198" t="s">
         <v>30</v>
@@ -18597,7 +18382,7 @@
         <v>Annual</v>
       </c>
       <c r="G12" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H12" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18616,7 +18401,7 @@
       </c>
       <c r="L12" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E4Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E4Y#0004</v>
       </c>
       <c r="M12" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -18627,7 +18412,7 @@
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="149"/>
       <c r="B13" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C13" s="198" t="s">
         <v>29</v>
@@ -18643,7 +18428,7 @@
         <v>Annual</v>
       </c>
       <c r="G13" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H13" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18662,7 +18447,7 @@
       </c>
       <c r="L13" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E5Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E5Y#0004</v>
       </c>
       <c r="M13" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -18673,7 +18458,7 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="149"/>
       <c r="B14" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C14" s="198" t="s">
         <v>28</v>
@@ -18689,7 +18474,7 @@
         <v>Annual</v>
       </c>
       <c r="G14" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H14" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18708,7 +18493,7 @@
       </c>
       <c r="L14" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E6Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E6Y#0004</v>
       </c>
       <c r="M14" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -18719,7 +18504,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="149"/>
       <c r="B15" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C15" s="198" t="s">
         <v>27</v>
@@ -18735,7 +18520,7 @@
         <v>Annual</v>
       </c>
       <c r="G15" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H15" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18754,7 +18539,7 @@
       </c>
       <c r="L15" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E7Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E7Y#0004</v>
       </c>
       <c r="M15" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -18765,7 +18550,7 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="149"/>
       <c r="B16" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C16" s="198" t="s">
         <v>26</v>
@@ -18781,7 +18566,7 @@
         <v>Annual</v>
       </c>
       <c r="G16" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H16" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18800,7 +18585,7 @@
       </c>
       <c r="L16" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E8Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E8Y#0004</v>
       </c>
       <c r="M16" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -18811,7 +18596,7 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="149"/>
       <c r="B17" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C17" s="198" t="s">
         <v>25</v>
@@ -18827,7 +18612,7 @@
         <v>Annual</v>
       </c>
       <c r="G17" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H17" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18846,7 +18631,7 @@
       </c>
       <c r="L17" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E9Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E9Y#0004</v>
       </c>
       <c r="M17" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -18857,7 +18642,7 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="149"/>
       <c r="B18" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C18" s="198" t="s">
         <v>24</v>
@@ -18873,7 +18658,7 @@
         <v>Annual</v>
       </c>
       <c r="G18" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H18" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18892,7 +18677,7 @@
       </c>
       <c r="L18" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E10Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E10Y#0004</v>
       </c>
       <c r="M18" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -18903,7 +18688,7 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="149"/>
       <c r="B19" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C19" s="198" t="s">
         <v>23</v>
@@ -18919,7 +18704,7 @@
         <v>Annual</v>
       </c>
       <c r="G19" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H19" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18938,7 +18723,7 @@
       </c>
       <c r="L19" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E11Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E11Y#0004</v>
       </c>
       <c r="M19" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -18949,7 +18734,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="149"/>
       <c r="B20" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C20" s="198" t="s">
         <v>22</v>
@@ -18965,7 +18750,7 @@
         <v>Annual</v>
       </c>
       <c r="G20" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H20" s="173" t="str">
         <f t="shared" si="3"/>
@@ -18984,7 +18769,7 @@
       </c>
       <c r="L20" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E12Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E12Y#0004</v>
       </c>
       <c r="M20" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -18995,7 +18780,7 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="149"/>
       <c r="B21" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C21" s="198" t="s">
         <v>21</v>
@@ -19011,7 +18796,7 @@
         <v>Annual</v>
       </c>
       <c r="G21" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H21" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19030,7 +18815,7 @@
       </c>
       <c r="L21" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E13Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E13Y#0004</v>
       </c>
       <c r="M21" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -19041,7 +18826,7 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="149"/>
       <c r="B22" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C22" s="198" t="s">
         <v>20</v>
@@ -19057,7 +18842,7 @@
         <v>Annual</v>
       </c>
       <c r="G22" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H22" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19076,7 +18861,7 @@
       </c>
       <c r="L22" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E14Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E14Y#0004</v>
       </c>
       <c r="M22" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -19087,7 +18872,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="149"/>
       <c r="B23" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C23" s="198" t="s">
         <v>19</v>
@@ -19103,7 +18888,7 @@
         <v>Annual</v>
       </c>
       <c r="G23" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H23" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19122,7 +18907,7 @@
       </c>
       <c r="L23" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E15Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E15Y#0004</v>
       </c>
       <c r="M23" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -19133,7 +18918,7 @@
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="149"/>
       <c r="B24" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C24" s="198" t="s">
         <v>18</v>
@@ -19149,7 +18934,7 @@
         <v>Annual</v>
       </c>
       <c r="G24" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H24" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19168,7 +18953,7 @@
       </c>
       <c r="L24" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E16Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E16Y#0004</v>
       </c>
       <c r="M24" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -19179,7 +18964,7 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="149"/>
       <c r="B25" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C25" s="198" t="s">
         <v>17</v>
@@ -19195,7 +18980,7 @@
         <v>Annual</v>
       </c>
       <c r="G25" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H25" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19214,7 +18999,7 @@
       </c>
       <c r="L25" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E17Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E17Y#0004</v>
       </c>
       <c r="M25" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -19225,7 +19010,7 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="149"/>
       <c r="B26" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C26" s="198" t="s">
         <v>16</v>
@@ -19241,7 +19026,7 @@
         <v>Annual</v>
       </c>
       <c r="G26" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H26" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19260,7 +19045,7 @@
       </c>
       <c r="L26" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E18Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E18Y#0004</v>
       </c>
       <c r="M26" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -19271,7 +19056,7 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="149"/>
       <c r="B27" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C27" s="198" t="s">
         <v>15</v>
@@ -19287,7 +19072,7 @@
         <v>Annual</v>
       </c>
       <c r="G27" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H27" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19306,7 +19091,7 @@
       </c>
       <c r="L27" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E19Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E19Y#0004</v>
       </c>
       <c r="M27" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -19317,7 +19102,7 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="149"/>
       <c r="B28" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C28" s="198" t="s">
         <v>14</v>
@@ -19333,7 +19118,7 @@
         <v>Annual</v>
       </c>
       <c r="G28" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H28" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19352,7 +19137,7 @@
       </c>
       <c r="L28" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E20Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E20Y#0004</v>
       </c>
       <c r="M28" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -19363,7 +19148,7 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="149"/>
       <c r="B29" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C29" s="198" t="s">
         <v>13</v>
@@ -19379,7 +19164,7 @@
         <v>Annual</v>
       </c>
       <c r="G29" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H29" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19398,7 +19183,7 @@
       </c>
       <c r="L29" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E21Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E21Y#0004</v>
       </c>
       <c r="M29" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -19409,7 +19194,7 @@
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="149"/>
       <c r="B30" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C30" s="198" t="s">
         <v>12</v>
@@ -19425,7 +19210,7 @@
         <v>Annual</v>
       </c>
       <c r="G30" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H30" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19444,7 +19229,7 @@
       </c>
       <c r="L30" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E22Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E22Y#0004</v>
       </c>
       <c r="M30" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -19455,7 +19240,7 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="149"/>
       <c r="B31" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C31" s="198" t="s">
         <v>11</v>
@@ -19471,7 +19256,7 @@
         <v>Annual</v>
       </c>
       <c r="G31" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H31" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19490,7 +19275,7 @@
       </c>
       <c r="L31" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E23Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E23Y#0004</v>
       </c>
       <c r="M31" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -19501,7 +19286,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="149"/>
       <c r="B32" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C32" s="198" t="s">
         <v>10</v>
@@ -19517,7 +19302,7 @@
         <v>Annual</v>
       </c>
       <c r="G32" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H32" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19536,7 +19321,7 @@
       </c>
       <c r="L32" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E24Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E24Y#0004</v>
       </c>
       <c r="M32" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -19547,7 +19332,7 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="149"/>
       <c r="B33" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C33" s="198" t="s">
         <v>9</v>
@@ -19563,7 +19348,7 @@
         <v>Annual</v>
       </c>
       <c r="G33" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H33" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19582,7 +19367,7 @@
       </c>
       <c r="L33" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E25Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E25Y#0004</v>
       </c>
       <c r="M33" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -19593,7 +19378,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="149"/>
       <c r="B34" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C34" s="198" t="s">
         <v>8</v>
@@ -19609,7 +19394,7 @@
         <v>Annual</v>
       </c>
       <c r="G34" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H34" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19628,7 +19413,7 @@
       </c>
       <c r="L34" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E26Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E26Y#0004</v>
       </c>
       <c r="M34" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -19639,7 +19424,7 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="149"/>
       <c r="B35" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C35" s="198" t="s">
         <v>7</v>
@@ -19655,7 +19440,7 @@
         <v>Annual</v>
       </c>
       <c r="G35" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H35" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19674,7 +19459,7 @@
       </c>
       <c r="L35" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E27Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E27Y#0004</v>
       </c>
       <c r="M35" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -19685,7 +19470,7 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="149"/>
       <c r="B36" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C36" s="198" t="s">
         <v>6</v>
@@ -19701,7 +19486,7 @@
         <v>Annual</v>
       </c>
       <c r="G36" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H36" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19720,7 +19505,7 @@
       </c>
       <c r="L36" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E28Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E28Y#0004</v>
       </c>
       <c r="M36" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -19731,7 +19516,7 @@
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="149"/>
       <c r="B37" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C37" s="198" t="s">
         <v>5</v>
@@ -19747,7 +19532,7 @@
         <v>Annual</v>
       </c>
       <c r="G37" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H37" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19766,7 +19551,7 @@
       </c>
       <c r="L37" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E29Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E29Y#0004</v>
       </c>
       <c r="M37" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -19777,7 +19562,7 @@
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="149"/>
       <c r="B38" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C38" s="198" t="s">
         <v>4</v>
@@ -19793,7 +19578,7 @@
         <v>Annual</v>
       </c>
       <c r="G38" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H38" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19812,7 +19597,7 @@
       </c>
       <c r="L38" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E30Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E30Y#0004</v>
       </c>
       <c r="M38" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -19823,7 +19608,7 @@
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="149"/>
       <c r="B39" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C39" s="198" t="s">
         <v>3</v>
@@ -19839,7 +19624,7 @@
         <v>Annual</v>
       </c>
       <c r="G39" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H39" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19858,7 +19643,7 @@
       </c>
       <c r="L39" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E35Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E35Y#0004</v>
       </c>
       <c r="M39" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -19869,7 +19654,7 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="149"/>
       <c r="B40" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C40" s="198" t="s">
         <v>2</v>
@@ -19885,7 +19670,7 @@
         <v>Annual</v>
       </c>
       <c r="G40" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H40" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19904,7 +19689,7 @@
       </c>
       <c r="L40" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E40Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E40Y#0004</v>
       </c>
       <c r="M40" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -19915,7 +19700,7 @@
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="149"/>
       <c r="B41" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C41" s="198" t="s">
         <v>1</v>
@@ -19931,7 +19716,7 @@
         <v>Annual</v>
       </c>
       <c r="G41" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H41" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19950,7 +19735,7 @@
       </c>
       <c r="L41" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E50Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E50Y#0004</v>
       </c>
       <c r="M41" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -19961,7 +19746,7 @@
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="149"/>
       <c r="B42" s="198" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C42" s="198" t="s">
         <v>0</v>
@@ -19977,7 +19762,7 @@
         <v>Annual</v>
       </c>
       <c r="G42" s="173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="H42" s="173" t="str">
         <f t="shared" si="3"/>
@@ -19996,7 +19781,7 @@
       </c>
       <c r="L42" s="194" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_AB6E60Y#0001</v>
+        <v>EUR_YCSTDRH_AB6E60Y#0004</v>
       </c>
       <c r="M42" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>